<commit_message>
updated meta and file contents
</commit_message>
<xml_diff>
--- a/corpus/evenki/current_meta.xlsx
+++ b/corpus/evenki/current_meta.xlsx
@@ -8,8 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$I$87</definedName>
     <definedName name="meta" localSheetId="0">Лист1!$A$1:$A$87</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="307">
   <si>
     <t>filename</t>
   </si>
@@ -908,13 +910,55 @@
   </si>
   <si>
     <t>http://siberian-lang.srcc.msu.ru/ru/text/ya-ohotilsya-na-losya-v-mukto</t>
+  </si>
+  <si>
+    <t>Сергеев Трофим Павлович</t>
+  </si>
+  <si>
+    <t>На Енчембу</t>
+  </si>
+  <si>
+    <t>Дикий олень</t>
+  </si>
+  <si>
+    <t>На Северной Таймуре</t>
+  </si>
+  <si>
+    <t>http://siberian-lang.srcc.msu.ru/ru/text/na-severnoy-taymure-s-m-andreeva</t>
+  </si>
+  <si>
+    <t>Конорёнок Марта Алексеевна</t>
+  </si>
+  <si>
+    <t>Суринда</t>
+  </si>
+  <si>
+    <t>Подготовка к аргишу</t>
+  </si>
+  <si>
+    <t>Лапушкина Марина Дмитриевна</t>
+  </si>
+  <si>
+    <t>Увачан Инна Константиновна</t>
+  </si>
+  <si>
+    <t>Я родился в лесу</t>
+  </si>
+  <si>
+    <t>Чемпогир Антонина Дмитриевна</t>
+  </si>
+  <si>
+    <t>http://siberian-lang.srcc.msu.ru/ru/text/rasskaz-o-zhizni-d-chempogir</t>
+  </si>
+  <si>
+    <t>В тундре</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -924,18 +968,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFDD1144"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -958,15 +1010,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1266,10 +1319,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="I87" sqref="I87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1280,36 +1334,36 @@
     <col min="9" max="9" width="59.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" hidden="1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1334,11 +1388,11 @@
       <c r="H2">
         <v>1998</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" hidden="1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1363,11 +1417,11 @@
       <c r="H3">
         <v>2005</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" hidden="1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1392,16 +1446,37 @@
       <c r="H4">
         <v>2005</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" hidden="1">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="B5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C5">
+        <v>2005</v>
+      </c>
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5">
+        <v>2005</v>
+      </c>
+      <c r="H5">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" hidden="1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1426,11 +1501,11 @@
       <c r="H6">
         <v>2006</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" hidden="1">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1455,11 +1530,11 @@
       <c r="H7">
         <v>2006</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" hidden="1">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1484,11 +1559,11 @@
       <c r="H8">
         <v>2006</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" hidden="1">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1513,11 +1588,11 @@
       <c r="H9">
         <v>2006</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" hidden="1">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1542,11 +1617,11 @@
       <c r="H10">
         <v>2006</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" hidden="1">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1571,11 +1646,11 @@
       <c r="H11">
         <v>2006</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" hidden="1">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1600,11 +1675,11 @@
       <c r="H12">
         <v>2007</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" hidden="1">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1629,11 +1704,11 @@
       <c r="H13">
         <v>2007</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" hidden="1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1658,11 +1733,11 @@
       <c r="H14">
         <v>2007</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" hidden="1">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1687,11 +1762,11 @@
       <c r="H15">
         <v>2007</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" hidden="1">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1716,11 +1791,11 @@
       <c r="H16">
         <v>2007</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" hidden="1">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1745,11 +1820,11 @@
       <c r="H17">
         <v>2007</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" hidden="1">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1774,11 +1849,11 @@
       <c r="H18">
         <v>2007</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" hidden="1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1803,11 +1878,11 @@
       <c r="H19">
         <v>2007</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" hidden="1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1832,11 +1907,11 @@
       <c r="H20">
         <v>2007</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" hidden="1">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1861,11 +1936,11 @@
       <c r="H21">
         <v>2007</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" hidden="1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1890,11 +1965,11 @@
       <c r="H22">
         <v>2007</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" hidden="1">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1919,11 +1994,11 @@
       <c r="H23">
         <v>2007</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I23" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" hidden="1">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1948,11 +2023,11 @@
       <c r="H24">
         <v>2007</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" hidden="1">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1977,11 +2052,11 @@
       <c r="H25">
         <v>2007</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I25" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" hidden="1">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2006,11 +2081,11 @@
       <c r="H26">
         <v>2007</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" hidden="1">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2035,11 +2110,11 @@
       <c r="H27">
         <v>2007</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I27" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" hidden="1">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2064,11 +2139,11 @@
       <c r="H28">
         <v>2007</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I28" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" hidden="1">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2093,11 +2168,11 @@
       <c r="H29">
         <v>2007</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="I29" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" hidden="1">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2122,11 +2197,11 @@
       <c r="H30">
         <v>2007</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" hidden="1">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2151,11 +2226,11 @@
       <c r="H31">
         <v>2007</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" hidden="1">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2180,11 +2255,11 @@
       <c r="H32">
         <v>2007</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" hidden="1">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2209,11 +2284,11 @@
       <c r="H33">
         <v>2007</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="I33" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" hidden="1">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2238,26 +2313,92 @@
       <c r="H34">
         <v>2007</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I34" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" hidden="1">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="B35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35">
+        <v>2007</v>
+      </c>
+      <c r="D35" t="s">
+        <v>175</v>
+      </c>
+      <c r="E35" t="s">
+        <v>294</v>
+      </c>
+      <c r="F35" t="s">
+        <v>105</v>
+      </c>
+      <c r="G35">
+        <v>2007</v>
+      </c>
+      <c r="H35">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" hidden="1">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="B36" t="s">
+        <v>174</v>
+      </c>
+      <c r="C36">
+        <v>2007</v>
+      </c>
+      <c r="D36" t="s">
+        <v>175</v>
+      </c>
+      <c r="E36" t="s">
+        <v>295</v>
+      </c>
+      <c r="F36" t="s">
+        <v>105</v>
+      </c>
+      <c r="G36">
+        <v>2007</v>
+      </c>
+      <c r="H36">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" hidden="1">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="B37" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37">
+        <v>2007</v>
+      </c>
+      <c r="D37" t="s">
+        <v>179</v>
+      </c>
+      <c r="E37" t="s">
+        <v>296</v>
+      </c>
+      <c r="F37" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37">
+        <v>2007</v>
+      </c>
+      <c r="H37">
+        <v>2007</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" hidden="1">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2282,11 +2423,11 @@
       <c r="H38">
         <v>2007</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="I38" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" hidden="1">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2311,11 +2452,11 @@
       <c r="H39">
         <v>2007</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="I39" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" hidden="1">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2340,11 +2481,11 @@
       <c r="H40">
         <v>2007</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I40" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" hidden="1">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2369,16 +2510,37 @@
       <c r="H41">
         <v>2007</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="I41" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" hidden="1">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="B42" t="s">
+        <v>298</v>
+      </c>
+      <c r="C42">
+        <v>2005</v>
+      </c>
+      <c r="D42" t="s">
+        <v>299</v>
+      </c>
+      <c r="E42" t="s">
+        <v>300</v>
+      </c>
+      <c r="F42" t="s">
+        <v>105</v>
+      </c>
+      <c r="G42">
+        <v>2005</v>
+      </c>
+      <c r="H42">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" hidden="1">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2403,11 +2565,11 @@
       <c r="H43">
         <v>2008</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="I43" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" hidden="1">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2432,11 +2594,11 @@
       <c r="H44">
         <v>2008</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="I44" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" hidden="1">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2461,11 +2623,11 @@
       <c r="H45">
         <v>2008</v>
       </c>
-      <c r="I45" s="2" t="s">
+      <c r="I45" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" hidden="1">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2490,11 +2652,11 @@
       <c r="H46">
         <v>2008</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="I46" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" hidden="1">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2519,11 +2681,11 @@
       <c r="H47">
         <v>2008</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="I47" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" hidden="1">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2548,11 +2710,11 @@
       <c r="H48">
         <v>2008</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="I48" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" hidden="1">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2577,11 +2739,11 @@
       <c r="H49">
         <v>2008</v>
       </c>
-      <c r="I49" s="2" t="s">
+      <c r="I49" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" hidden="1">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2606,11 +2768,11 @@
       <c r="H50">
         <v>2008</v>
       </c>
-      <c r="I50" s="2" t="s">
+      <c r="I50" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" hidden="1">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2635,11 +2797,11 @@
       <c r="H51">
         <v>2008</v>
       </c>
-      <c r="I51" s="2" t="s">
+      <c r="I51" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" hidden="1">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2664,11 +2826,11 @@
       <c r="H52">
         <v>2008</v>
       </c>
-      <c r="I52" s="2" t="s">
+      <c r="I52" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" hidden="1">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2693,11 +2855,11 @@
       <c r="H53">
         <v>2008</v>
       </c>
-      <c r="I53" s="2" t="s">
+      <c r="I53" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" hidden="1">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2722,11 +2884,11 @@
       <c r="H54">
         <v>2008</v>
       </c>
-      <c r="I54" s="2" t="s">
+      <c r="I54" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" hidden="1">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2751,11 +2913,11 @@
       <c r="H55">
         <v>2008</v>
       </c>
-      <c r="I55" s="2" t="s">
+      <c r="I55" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" hidden="1">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2780,16 +2942,37 @@
       <c r="H56">
         <v>2008</v>
       </c>
-      <c r="I56" s="2" t="s">
+      <c r="I56" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" hidden="1">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="B57" t="s">
+        <v>301</v>
+      </c>
+      <c r="C57">
+        <v>2008</v>
+      </c>
+      <c r="D57" t="s">
+        <v>216</v>
+      </c>
+      <c r="E57" t="s">
+        <v>98</v>
+      </c>
+      <c r="F57" t="s">
+        <v>105</v>
+      </c>
+      <c r="G57">
+        <v>2008</v>
+      </c>
+      <c r="H57">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" hidden="1">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2814,27 +2997,90 @@
       <c r="H58">
         <v>2008</v>
       </c>
-      <c r="I58" s="2" t="s">
+      <c r="I58" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" hidden="1">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="I59" s="2"/>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="B59" t="s">
+        <v>302</v>
+      </c>
+      <c r="C59">
+        <v>2008</v>
+      </c>
+      <c r="D59" t="s">
+        <v>216</v>
+      </c>
+      <c r="E59" t="s">
+        <v>98</v>
+      </c>
+      <c r="F59" t="s">
+        <v>105</v>
+      </c>
+      <c r="G59">
+        <v>2008</v>
+      </c>
+      <c r="H59">
+        <v>2008</v>
+      </c>
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="1:9" hidden="1">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="B60" t="s">
+        <v>302</v>
+      </c>
+      <c r="C60">
+        <v>2008</v>
+      </c>
+      <c r="D60" t="s">
+        <v>216</v>
+      </c>
+      <c r="E60" t="s">
+        <v>98</v>
+      </c>
+      <c r="F60" t="s">
+        <v>105</v>
+      </c>
+      <c r="G60">
+        <v>2008</v>
+      </c>
+      <c r="H60">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" hidden="1">
       <c r="A61" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="B61" t="s">
+        <v>302</v>
+      </c>
+      <c r="C61">
+        <v>2008</v>
+      </c>
+      <c r="D61" t="s">
+        <v>216</v>
+      </c>
+      <c r="E61" t="s">
+        <v>98</v>
+      </c>
+      <c r="F61" t="s">
+        <v>105</v>
+      </c>
+      <c r="G61">
+        <v>2008</v>
+      </c>
+      <c r="H61">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" hidden="1">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2859,11 +3105,11 @@
       <c r="H62">
         <v>2009</v>
       </c>
-      <c r="I62" s="2" t="s">
+      <c r="I62" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" hidden="1">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2888,16 +3134,37 @@
       <c r="H63">
         <v>2009</v>
       </c>
-      <c r="I63" s="2" t="s">
+      <c r="I63" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" hidden="1">
       <c r="A64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="B64" t="s">
+        <v>233</v>
+      </c>
+      <c r="C64">
+        <v>2010</v>
+      </c>
+      <c r="D64" t="s">
+        <v>234</v>
+      </c>
+      <c r="E64" t="s">
+        <v>303</v>
+      </c>
+      <c r="F64" t="s">
+        <v>105</v>
+      </c>
+      <c r="G64">
+        <v>2010</v>
+      </c>
+      <c r="H64">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" hidden="1">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2922,7 +3189,7 @@
       <c r="H65">
         <v>2010</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="I65" s="1" t="s">
         <v>236</v>
       </c>
     </row>
@@ -2931,17 +3198,62 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" hidden="1">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="B67" t="s">
+        <v>304</v>
+      </c>
+      <c r="C67">
+        <v>2011</v>
+      </c>
+      <c r="D67" t="s">
+        <v>237</v>
+      </c>
+      <c r="E67" t="s">
+        <v>98</v>
+      </c>
+      <c r="F67" t="s">
+        <v>105</v>
+      </c>
+      <c r="G67">
+        <v>2011</v>
+      </c>
+      <c r="H67">
+        <v>2011</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" hidden="1">
       <c r="A68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="B68" t="s">
+        <v>304</v>
+      </c>
+      <c r="C68">
+        <v>2011</v>
+      </c>
+      <c r="D68" t="s">
+        <v>237</v>
+      </c>
+      <c r="E68" t="s">
+        <v>306</v>
+      </c>
+      <c r="F68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G68">
+        <v>2011</v>
+      </c>
+      <c r="H68">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" hidden="1">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2966,11 +3278,11 @@
       <c r="H69">
         <v>2011</v>
       </c>
-      <c r="I69" s="2" t="s">
+      <c r="I69" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" hidden="1">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2995,11 +3307,11 @@
       <c r="H70">
         <v>2011</v>
       </c>
-      <c r="I70" s="2" t="s">
+      <c r="I70" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" hidden="1">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -3024,11 +3336,11 @@
       <c r="H71">
         <v>2011</v>
       </c>
-      <c r="I71" s="2" t="s">
+      <c r="I71" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" hidden="1">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -3053,11 +3365,11 @@
       <c r="H72">
         <v>2014</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="I72" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" hidden="1">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -3082,11 +3394,11 @@
       <c r="H73">
         <v>2014</v>
       </c>
-      <c r="I73" s="2" t="s">
+      <c r="I73" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" hidden="1">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -3111,11 +3423,11 @@
       <c r="H74">
         <v>2014</v>
       </c>
-      <c r="I74" s="2" t="s">
+      <c r="I74" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" hidden="1">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -3140,11 +3452,11 @@
       <c r="H75">
         <v>2014</v>
       </c>
-      <c r="I75" s="2" t="s">
+      <c r="I75" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" hidden="1">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -3169,11 +3481,11 @@
       <c r="H76">
         <v>2014</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="I76" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" hidden="1">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -3198,11 +3510,11 @@
       <c r="H77">
         <v>2016</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="I77" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" hidden="1">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -3227,11 +3539,11 @@
       <c r="H78">
         <v>2016</v>
       </c>
-      <c r="I78" s="2" t="s">
+      <c r="I78" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" hidden="1">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -3256,11 +3568,11 @@
       <c r="H79">
         <v>2016</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="I79" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" hidden="1">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -3285,11 +3597,11 @@
       <c r="H80">
         <v>1952</v>
       </c>
-      <c r="I80" s="2" t="s">
+      <c r="I80" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" hidden="1">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -3314,11 +3626,11 @@
       <c r="H81">
         <v>1952</v>
       </c>
-      <c r="I81" s="2" t="s">
+      <c r="I81" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" hidden="1">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -3343,11 +3655,11 @@
       <c r="H82">
         <v>1952</v>
       </c>
-      <c r="I82" s="2" t="s">
+      <c r="I82" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" hidden="1">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -3372,11 +3684,11 @@
       <c r="H83">
         <v>1952</v>
       </c>
-      <c r="I83" s="2" t="s">
+      <c r="I83" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" hidden="1">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -3401,11 +3713,11 @@
       <c r="H84">
         <v>1952</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="I84" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" hidden="1">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -3430,11 +3742,11 @@
       <c r="H85">
         <v>1952</v>
       </c>
-      <c r="I85" s="2" t="s">
+      <c r="I85" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" hidden="1">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -3459,11 +3771,11 @@
       <c r="H86">
         <v>1952</v>
       </c>
-      <c r="I86" s="2" t="s">
+      <c r="I86" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" hidden="1">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -3488,11 +3800,16 @@
       <c r="H87">
         <v>1952</v>
       </c>
-      <c r="I87" s="2" t="s">
+      <c r="I87" s="1" t="s">
         <v>292</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I87">
+    <filterColumn colId="1">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
     <hyperlink ref="I3" r:id="rId2"/>
@@ -3567,8 +3884,2497 @@
     <hyperlink ref="I85" r:id="rId71"/>
     <hyperlink ref="I86" r:id="rId72"/>
     <hyperlink ref="I87" r:id="rId73"/>
+    <hyperlink ref="I37" r:id="rId74"/>
+    <hyperlink ref="I67" r:id="rId75"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId74"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId76"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I87"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="68.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2">
+        <v>1998</v>
+      </c>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2">
+        <v>1998</v>
+      </c>
+      <c r="H2">
+        <v>1998</v>
+      </c>
+      <c r="I2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3">
+        <v>2005</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3">
+        <v>2005</v>
+      </c>
+      <c r="H3">
+        <v>2005</v>
+      </c>
+      <c r="I3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4">
+        <v>2005</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4">
+        <v>2005</v>
+      </c>
+      <c r="H4">
+        <v>2005</v>
+      </c>
+      <c r="I4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C5">
+        <v>2005</v>
+      </c>
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5">
+        <v>2005</v>
+      </c>
+      <c r="H5">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6">
+        <v>2006</v>
+      </c>
+      <c r="D6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6">
+        <v>2006</v>
+      </c>
+      <c r="H6">
+        <v>2006</v>
+      </c>
+      <c r="I6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7">
+        <v>2006</v>
+      </c>
+      <c r="D7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7">
+        <v>2006</v>
+      </c>
+      <c r="H7">
+        <v>2006</v>
+      </c>
+      <c r="I7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8">
+        <v>2006</v>
+      </c>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8">
+        <v>2006</v>
+      </c>
+      <c r="H8">
+        <v>2006</v>
+      </c>
+      <c r="I8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9">
+        <v>2006</v>
+      </c>
+      <c r="D9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9">
+        <v>2006</v>
+      </c>
+      <c r="H9">
+        <v>2006</v>
+      </c>
+      <c r="I9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10">
+        <v>2006</v>
+      </c>
+      <c r="D10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10">
+        <v>2006</v>
+      </c>
+      <c r="H10">
+        <v>2006</v>
+      </c>
+      <c r="I10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11">
+        <v>2006</v>
+      </c>
+      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11">
+        <v>2006</v>
+      </c>
+      <c r="H11">
+        <v>2006</v>
+      </c>
+      <c r="I11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12">
+        <v>2007</v>
+      </c>
+      <c r="D12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F12" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12">
+        <v>2007</v>
+      </c>
+      <c r="H12">
+        <v>2007</v>
+      </c>
+      <c r="I12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13">
+        <v>2007</v>
+      </c>
+      <c r="D13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13">
+        <v>2007</v>
+      </c>
+      <c r="H13">
+        <v>2007</v>
+      </c>
+      <c r="I13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14">
+        <v>2007</v>
+      </c>
+      <c r="D14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14">
+        <v>2007</v>
+      </c>
+      <c r="H14">
+        <v>2007</v>
+      </c>
+      <c r="I14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15">
+        <v>2007</v>
+      </c>
+      <c r="D15" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G15">
+        <v>2007</v>
+      </c>
+      <c r="H15">
+        <v>2007</v>
+      </c>
+      <c r="I15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16">
+        <v>2007</v>
+      </c>
+      <c r="D16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16">
+        <v>2007</v>
+      </c>
+      <c r="H16">
+        <v>2007</v>
+      </c>
+      <c r="I16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17">
+        <v>2007</v>
+      </c>
+      <c r="D17" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" t="s">
+        <v>148</v>
+      </c>
+      <c r="F17" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17">
+        <v>2007</v>
+      </c>
+      <c r="H17">
+        <v>2007</v>
+      </c>
+      <c r="I17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18">
+        <v>2007</v>
+      </c>
+      <c r="D18" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18">
+        <v>2007</v>
+      </c>
+      <c r="H18">
+        <v>2007</v>
+      </c>
+      <c r="I18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19">
+        <v>2007</v>
+      </c>
+      <c r="D19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19">
+        <v>2007</v>
+      </c>
+      <c r="H19">
+        <v>2007</v>
+      </c>
+      <c r="I19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20">
+        <v>2007</v>
+      </c>
+      <c r="D20" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20">
+        <v>2007</v>
+      </c>
+      <c r="H20">
+        <v>2007</v>
+      </c>
+      <c r="I20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21">
+        <v>2007</v>
+      </c>
+      <c r="D21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21">
+        <v>2007</v>
+      </c>
+      <c r="H21">
+        <v>2007</v>
+      </c>
+      <c r="I21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22">
+        <v>2007</v>
+      </c>
+      <c r="D22" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" t="s">
+        <v>155</v>
+      </c>
+      <c r="F22" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22">
+        <v>2007</v>
+      </c>
+      <c r="H22">
+        <v>2007</v>
+      </c>
+      <c r="I22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23">
+        <v>2007</v>
+      </c>
+      <c r="D23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" t="s">
+        <v>126</v>
+      </c>
+      <c r="G23">
+        <v>2007</v>
+      </c>
+      <c r="H23">
+        <v>2007</v>
+      </c>
+      <c r="I23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24">
+        <v>2007</v>
+      </c>
+      <c r="D24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" t="s">
+        <v>130</v>
+      </c>
+      <c r="F24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24">
+        <v>2007</v>
+      </c>
+      <c r="H24">
+        <v>2007</v>
+      </c>
+      <c r="I24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25">
+        <v>2007</v>
+      </c>
+      <c r="D25" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" t="s">
+        <v>132</v>
+      </c>
+      <c r="F25" t="s">
+        <v>126</v>
+      </c>
+      <c r="G25">
+        <v>2007</v>
+      </c>
+      <c r="H25">
+        <v>2007</v>
+      </c>
+      <c r="I25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26">
+        <v>2007</v>
+      </c>
+      <c r="D26" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" t="s">
+        <v>145</v>
+      </c>
+      <c r="F26" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26">
+        <v>2007</v>
+      </c>
+      <c r="H26">
+        <v>2007</v>
+      </c>
+      <c r="I26" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27">
+        <v>2007</v>
+      </c>
+      <c r="D27" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" t="s">
+        <v>143</v>
+      </c>
+      <c r="F27" t="s">
+        <v>105</v>
+      </c>
+      <c r="G27">
+        <v>2007</v>
+      </c>
+      <c r="H27">
+        <v>2007</v>
+      </c>
+      <c r="I27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28">
+        <v>2007</v>
+      </c>
+      <c r="D28" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28">
+        <v>2007</v>
+      </c>
+      <c r="H28">
+        <v>2007</v>
+      </c>
+      <c r="I28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29">
+        <v>2007</v>
+      </c>
+      <c r="D29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" t="s">
+        <v>161</v>
+      </c>
+      <c r="F29" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29">
+        <v>2007</v>
+      </c>
+      <c r="H29">
+        <v>2007</v>
+      </c>
+      <c r="I29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30">
+        <v>2007</v>
+      </c>
+      <c r="D30" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30">
+        <v>2007</v>
+      </c>
+      <c r="H30">
+        <v>2007</v>
+      </c>
+      <c r="I30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>165</v>
+      </c>
+      <c r="C31">
+        <v>2007</v>
+      </c>
+      <c r="D31" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31">
+        <v>2007</v>
+      </c>
+      <c r="H31">
+        <v>2007</v>
+      </c>
+      <c r="I31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>170</v>
+      </c>
+      <c r="C32">
+        <v>2007</v>
+      </c>
+      <c r="D32" t="s">
+        <v>166</v>
+      </c>
+      <c r="E32" t="s">
+        <v>168</v>
+      </c>
+      <c r="F32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G32">
+        <v>2007</v>
+      </c>
+      <c r="H32">
+        <v>2007</v>
+      </c>
+      <c r="I32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>171</v>
+      </c>
+      <c r="C33">
+        <v>2007</v>
+      </c>
+      <c r="D33" t="s">
+        <v>166</v>
+      </c>
+      <c r="E33" t="s">
+        <v>172</v>
+      </c>
+      <c r="F33" t="s">
+        <v>126</v>
+      </c>
+      <c r="G33">
+        <v>2007</v>
+      </c>
+      <c r="H33">
+        <v>2007</v>
+      </c>
+      <c r="I33" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34">
+        <v>2007</v>
+      </c>
+      <c r="D34" t="s">
+        <v>175</v>
+      </c>
+      <c r="E34" t="s">
+        <v>176</v>
+      </c>
+      <c r="F34" t="s">
+        <v>105</v>
+      </c>
+      <c r="G34">
+        <v>2007</v>
+      </c>
+      <c r="H34">
+        <v>2007</v>
+      </c>
+      <c r="I34" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35">
+        <v>2007</v>
+      </c>
+      <c r="D35" t="s">
+        <v>175</v>
+      </c>
+      <c r="E35" t="s">
+        <v>294</v>
+      </c>
+      <c r="F35" t="s">
+        <v>105</v>
+      </c>
+      <c r="G35">
+        <v>2007</v>
+      </c>
+      <c r="H35">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>174</v>
+      </c>
+      <c r="C36">
+        <v>2007</v>
+      </c>
+      <c r="D36" t="s">
+        <v>175</v>
+      </c>
+      <c r="E36" t="s">
+        <v>295</v>
+      </c>
+      <c r="F36" t="s">
+        <v>105</v>
+      </c>
+      <c r="G36">
+        <v>2007</v>
+      </c>
+      <c r="H36">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37">
+        <v>2007</v>
+      </c>
+      <c r="D37" t="s">
+        <v>179</v>
+      </c>
+      <c r="E37" t="s">
+        <v>296</v>
+      </c>
+      <c r="F37" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37">
+        <v>2007</v>
+      </c>
+      <c r="H37">
+        <v>2007</v>
+      </c>
+      <c r="I37" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38">
+        <v>2007</v>
+      </c>
+      <c r="D38" t="s">
+        <v>179</v>
+      </c>
+      <c r="E38" t="s">
+        <v>182</v>
+      </c>
+      <c r="F38" t="s">
+        <v>105</v>
+      </c>
+      <c r="G38">
+        <v>2007</v>
+      </c>
+      <c r="H38">
+        <v>2007</v>
+      </c>
+      <c r="I38" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>178</v>
+      </c>
+      <c r="C39">
+        <v>2007</v>
+      </c>
+      <c r="D39" t="s">
+        <v>179</v>
+      </c>
+      <c r="E39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F39" t="s">
+        <v>105</v>
+      </c>
+      <c r="G39">
+        <v>2007</v>
+      </c>
+      <c r="H39">
+        <v>2007</v>
+      </c>
+      <c r="I39" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>184</v>
+      </c>
+      <c r="C40">
+        <v>2007</v>
+      </c>
+      <c r="D40" t="s">
+        <v>179</v>
+      </c>
+      <c r="E40" t="s">
+        <v>185</v>
+      </c>
+      <c r="F40" t="s">
+        <v>105</v>
+      </c>
+      <c r="G40">
+        <v>2007</v>
+      </c>
+      <c r="H40">
+        <v>2007</v>
+      </c>
+      <c r="I40" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>184</v>
+      </c>
+      <c r="C41">
+        <v>2007</v>
+      </c>
+      <c r="D41" t="s">
+        <v>179</v>
+      </c>
+      <c r="E41" t="s">
+        <v>187</v>
+      </c>
+      <c r="F41" t="s">
+        <v>105</v>
+      </c>
+      <c r="G41">
+        <v>2007</v>
+      </c>
+      <c r="H41">
+        <v>2007</v>
+      </c>
+      <c r="I41" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>298</v>
+      </c>
+      <c r="C42">
+        <v>2005</v>
+      </c>
+      <c r="D42" t="s">
+        <v>299</v>
+      </c>
+      <c r="E42" t="s">
+        <v>300</v>
+      </c>
+      <c r="F42" t="s">
+        <v>105</v>
+      </c>
+      <c r="G42">
+        <v>2005</v>
+      </c>
+      <c r="H42">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43">
+        <v>2008</v>
+      </c>
+      <c r="D43" t="s">
+        <v>190</v>
+      </c>
+      <c r="E43" t="s">
+        <v>98</v>
+      </c>
+      <c r="F43" t="s">
+        <v>105</v>
+      </c>
+      <c r="G43">
+        <v>2008</v>
+      </c>
+      <c r="H43">
+        <v>2008</v>
+      </c>
+      <c r="I43" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>192</v>
+      </c>
+      <c r="C44">
+        <v>2008</v>
+      </c>
+      <c r="D44" t="s">
+        <v>190</v>
+      </c>
+      <c r="E44" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" t="s">
+        <v>105</v>
+      </c>
+      <c r="G44">
+        <v>2008</v>
+      </c>
+      <c r="H44">
+        <v>2008</v>
+      </c>
+      <c r="I44" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>196</v>
+      </c>
+      <c r="C45">
+        <v>2008</v>
+      </c>
+      <c r="D45" t="s">
+        <v>190</v>
+      </c>
+      <c r="E45" t="s">
+        <v>98</v>
+      </c>
+      <c r="F45" t="s">
+        <v>105</v>
+      </c>
+      <c r="G45">
+        <v>2008</v>
+      </c>
+      <c r="H45">
+        <v>2008</v>
+      </c>
+      <c r="I45" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>196</v>
+      </c>
+      <c r="C46">
+        <v>2008</v>
+      </c>
+      <c r="D46" t="s">
+        <v>190</v>
+      </c>
+      <c r="E46" t="s">
+        <v>194</v>
+      </c>
+      <c r="F46" t="s">
+        <v>105</v>
+      </c>
+      <c r="G46">
+        <v>2008</v>
+      </c>
+      <c r="H46">
+        <v>2008</v>
+      </c>
+      <c r="I46" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>196</v>
+      </c>
+      <c r="C47">
+        <v>2008</v>
+      </c>
+      <c r="D47" t="s">
+        <v>190</v>
+      </c>
+      <c r="E47" t="s">
+        <v>198</v>
+      </c>
+      <c r="F47" t="s">
+        <v>105</v>
+      </c>
+      <c r="G47">
+        <v>2008</v>
+      </c>
+      <c r="H47">
+        <v>2008</v>
+      </c>
+      <c r="I47" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>200</v>
+      </c>
+      <c r="C48">
+        <v>2008</v>
+      </c>
+      <c r="D48" t="s">
+        <v>201</v>
+      </c>
+      <c r="E48" t="s">
+        <v>202</v>
+      </c>
+      <c r="F48" t="s">
+        <v>105</v>
+      </c>
+      <c r="G48">
+        <v>2008</v>
+      </c>
+      <c r="H48">
+        <v>2008</v>
+      </c>
+      <c r="I48" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>200</v>
+      </c>
+      <c r="C49">
+        <v>2008</v>
+      </c>
+      <c r="D49" t="s">
+        <v>201</v>
+      </c>
+      <c r="E49" t="s">
+        <v>204</v>
+      </c>
+      <c r="F49" t="s">
+        <v>105</v>
+      </c>
+      <c r="G49">
+        <v>2008</v>
+      </c>
+      <c r="H49">
+        <v>2008</v>
+      </c>
+      <c r="I49" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>206</v>
+      </c>
+      <c r="C50">
+        <v>2008</v>
+      </c>
+      <c r="D50" t="s">
+        <v>201</v>
+      </c>
+      <c r="E50" t="s">
+        <v>211</v>
+      </c>
+      <c r="F50" t="s">
+        <v>126</v>
+      </c>
+      <c r="G50">
+        <v>2008</v>
+      </c>
+      <c r="H50">
+        <v>2008</v>
+      </c>
+      <c r="I50" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>206</v>
+      </c>
+      <c r="C51">
+        <v>2008</v>
+      </c>
+      <c r="D51" t="s">
+        <v>201</v>
+      </c>
+      <c r="E51" t="s">
+        <v>213</v>
+      </c>
+      <c r="F51" t="s">
+        <v>126</v>
+      </c>
+      <c r="G51">
+        <v>2008</v>
+      </c>
+      <c r="H51">
+        <v>2008</v>
+      </c>
+      <c r="I51" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>206</v>
+      </c>
+      <c r="C52">
+        <v>2008</v>
+      </c>
+      <c r="D52" t="s">
+        <v>201</v>
+      </c>
+      <c r="E52" t="s">
+        <v>209</v>
+      </c>
+      <c r="F52" t="s">
+        <v>126</v>
+      </c>
+      <c r="G52">
+        <v>2008</v>
+      </c>
+      <c r="H52">
+        <v>2008</v>
+      </c>
+      <c r="I52" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>206</v>
+      </c>
+      <c r="C53">
+        <v>2008</v>
+      </c>
+      <c r="D53" t="s">
+        <v>201</v>
+      </c>
+      <c r="E53" t="s">
+        <v>207</v>
+      </c>
+      <c r="F53" t="s">
+        <v>105</v>
+      </c>
+      <c r="G53">
+        <v>2008</v>
+      </c>
+      <c r="H53">
+        <v>2008</v>
+      </c>
+      <c r="I53" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>215</v>
+      </c>
+      <c r="C54">
+        <v>2008</v>
+      </c>
+      <c r="D54" t="s">
+        <v>216</v>
+      </c>
+      <c r="E54" t="s">
+        <v>217</v>
+      </c>
+      <c r="F54" t="s">
+        <v>105</v>
+      </c>
+      <c r="G54">
+        <v>2008</v>
+      </c>
+      <c r="H54">
+        <v>2008</v>
+      </c>
+      <c r="I54" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>219</v>
+      </c>
+      <c r="C55">
+        <v>2008</v>
+      </c>
+      <c r="D55" t="s">
+        <v>216</v>
+      </c>
+      <c r="E55" t="s">
+        <v>98</v>
+      </c>
+      <c r="F55" t="s">
+        <v>105</v>
+      </c>
+      <c r="G55">
+        <v>2008</v>
+      </c>
+      <c r="H55">
+        <v>2008</v>
+      </c>
+      <c r="I55" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>221</v>
+      </c>
+      <c r="C56">
+        <v>2008</v>
+      </c>
+      <c r="D56" t="s">
+        <v>216</v>
+      </c>
+      <c r="E56" t="s">
+        <v>222</v>
+      </c>
+      <c r="F56" t="s">
+        <v>105</v>
+      </c>
+      <c r="G56">
+        <v>2008</v>
+      </c>
+      <c r="H56">
+        <v>2008</v>
+      </c>
+      <c r="I56" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>301</v>
+      </c>
+      <c r="C57">
+        <v>2008</v>
+      </c>
+      <c r="D57" t="s">
+        <v>216</v>
+      </c>
+      <c r="E57" t="s">
+        <v>98</v>
+      </c>
+      <c r="F57" t="s">
+        <v>105</v>
+      </c>
+      <c r="G57">
+        <v>2008</v>
+      </c>
+      <c r="H57">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>224</v>
+      </c>
+      <c r="C58">
+        <v>2008</v>
+      </c>
+      <c r="D58" t="s">
+        <v>216</v>
+      </c>
+      <c r="E58" t="s">
+        <v>225</v>
+      </c>
+      <c r="F58" t="s">
+        <v>126</v>
+      </c>
+      <c r="G58">
+        <v>2008</v>
+      </c>
+      <c r="H58">
+        <v>2008</v>
+      </c>
+      <c r="I58" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>302</v>
+      </c>
+      <c r="C59">
+        <v>2008</v>
+      </c>
+      <c r="D59" t="s">
+        <v>216</v>
+      </c>
+      <c r="E59" t="s">
+        <v>98</v>
+      </c>
+      <c r="F59" t="s">
+        <v>105</v>
+      </c>
+      <c r="G59">
+        <v>2008</v>
+      </c>
+      <c r="H59">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>302</v>
+      </c>
+      <c r="C60">
+        <v>2008</v>
+      </c>
+      <c r="D60" t="s">
+        <v>216</v>
+      </c>
+      <c r="E60" t="s">
+        <v>98</v>
+      </c>
+      <c r="F60" t="s">
+        <v>105</v>
+      </c>
+      <c r="G60">
+        <v>2008</v>
+      </c>
+      <c r="H60">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>302</v>
+      </c>
+      <c r="C61">
+        <v>2008</v>
+      </c>
+      <c r="D61" t="s">
+        <v>216</v>
+      </c>
+      <c r="E61" t="s">
+        <v>98</v>
+      </c>
+      <c r="F61" t="s">
+        <v>105</v>
+      </c>
+      <c r="G61">
+        <v>2008</v>
+      </c>
+      <c r="H61">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>227</v>
+      </c>
+      <c r="C62">
+        <v>2009</v>
+      </c>
+      <c r="D62" t="s">
+        <v>228</v>
+      </c>
+      <c r="E62" t="s">
+        <v>229</v>
+      </c>
+      <c r="F62" t="s">
+        <v>105</v>
+      </c>
+      <c r="G62">
+        <v>2009</v>
+      </c>
+      <c r="H62">
+        <v>2009</v>
+      </c>
+      <c r="I62" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>227</v>
+      </c>
+      <c r="C63">
+        <v>2009</v>
+      </c>
+      <c r="D63" t="s">
+        <v>228</v>
+      </c>
+      <c r="E63" t="s">
+        <v>231</v>
+      </c>
+      <c r="F63" t="s">
+        <v>105</v>
+      </c>
+      <c r="G63">
+        <v>2009</v>
+      </c>
+      <c r="H63">
+        <v>2009</v>
+      </c>
+      <c r="I63" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>233</v>
+      </c>
+      <c r="C64">
+        <v>2010</v>
+      </c>
+      <c r="D64" t="s">
+        <v>234</v>
+      </c>
+      <c r="E64" t="s">
+        <v>303</v>
+      </c>
+      <c r="F64" t="s">
+        <v>105</v>
+      </c>
+      <c r="G64">
+        <v>2010</v>
+      </c>
+      <c r="H64">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>233</v>
+      </c>
+      <c r="C65">
+        <v>2010</v>
+      </c>
+      <c r="D65" t="s">
+        <v>234</v>
+      </c>
+      <c r="E65" t="s">
+        <v>235</v>
+      </c>
+      <c r="F65" t="s">
+        <v>105</v>
+      </c>
+      <c r="G65">
+        <v>2010</v>
+      </c>
+      <c r="H65">
+        <v>2010</v>
+      </c>
+      <c r="I65" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>304</v>
+      </c>
+      <c r="C67">
+        <v>2011</v>
+      </c>
+      <c r="D67" t="s">
+        <v>237</v>
+      </c>
+      <c r="E67" t="s">
+        <v>98</v>
+      </c>
+      <c r="F67" t="s">
+        <v>105</v>
+      </c>
+      <c r="G67">
+        <v>2011</v>
+      </c>
+      <c r="H67">
+        <v>2011</v>
+      </c>
+      <c r="I67" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>304</v>
+      </c>
+      <c r="C68">
+        <v>2011</v>
+      </c>
+      <c r="D68" t="s">
+        <v>237</v>
+      </c>
+      <c r="E68" t="s">
+        <v>306</v>
+      </c>
+      <c r="F68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G68">
+        <v>2011</v>
+      </c>
+      <c r="H68">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>238</v>
+      </c>
+      <c r="C69">
+        <v>2011</v>
+      </c>
+      <c r="D69" t="s">
+        <v>237</v>
+      </c>
+      <c r="E69" t="s">
+        <v>239</v>
+      </c>
+      <c r="F69" t="s">
+        <v>105</v>
+      </c>
+      <c r="G69">
+        <v>2011</v>
+      </c>
+      <c r="H69">
+        <v>2011</v>
+      </c>
+      <c r="I69" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>238</v>
+      </c>
+      <c r="C70">
+        <v>2011</v>
+      </c>
+      <c r="D70" t="s">
+        <v>237</v>
+      </c>
+      <c r="E70" t="s">
+        <v>98</v>
+      </c>
+      <c r="F70" t="s">
+        <v>105</v>
+      </c>
+      <c r="G70">
+        <v>2011</v>
+      </c>
+      <c r="H70">
+        <v>2011</v>
+      </c>
+      <c r="I70" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>242</v>
+      </c>
+      <c r="C71">
+        <v>2011</v>
+      </c>
+      <c r="D71" t="s">
+        <v>243</v>
+      </c>
+      <c r="E71" t="s">
+        <v>244</v>
+      </c>
+      <c r="F71" t="s">
+        <v>126</v>
+      </c>
+      <c r="G71">
+        <v>2011</v>
+      </c>
+      <c r="H71">
+        <v>2011</v>
+      </c>
+      <c r="I71" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>246</v>
+      </c>
+      <c r="C72">
+        <v>2014</v>
+      </c>
+      <c r="D72" t="s">
+        <v>201</v>
+      </c>
+      <c r="E72" t="s">
+        <v>247</v>
+      </c>
+      <c r="F72" t="s">
+        <v>105</v>
+      </c>
+      <c r="G72">
+        <v>2014</v>
+      </c>
+      <c r="H72">
+        <v>2014</v>
+      </c>
+      <c r="I72" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>249</v>
+      </c>
+      <c r="C73">
+        <v>2014</v>
+      </c>
+      <c r="D73" t="s">
+        <v>250</v>
+      </c>
+      <c r="E73" t="s">
+        <v>251</v>
+      </c>
+      <c r="F73" t="s">
+        <v>105</v>
+      </c>
+      <c r="G73">
+        <v>2014</v>
+      </c>
+      <c r="H73">
+        <v>2014</v>
+      </c>
+      <c r="I73" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>253</v>
+      </c>
+      <c r="C74">
+        <v>2014</v>
+      </c>
+      <c r="D74" t="s">
+        <v>254</v>
+      </c>
+      <c r="E74" t="s">
+        <v>255</v>
+      </c>
+      <c r="F74" t="s">
+        <v>126</v>
+      </c>
+      <c r="G74">
+        <v>2014</v>
+      </c>
+      <c r="H74">
+        <v>2014</v>
+      </c>
+      <c r="I74" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>253</v>
+      </c>
+      <c r="C75">
+        <v>2014</v>
+      </c>
+      <c r="D75" t="s">
+        <v>254</v>
+      </c>
+      <c r="E75" t="s">
+        <v>259</v>
+      </c>
+      <c r="F75" t="s">
+        <v>105</v>
+      </c>
+      <c r="G75">
+        <v>2014</v>
+      </c>
+      <c r="H75">
+        <v>2014</v>
+      </c>
+      <c r="I75" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>253</v>
+      </c>
+      <c r="C76">
+        <v>2014</v>
+      </c>
+      <c r="D76" t="s">
+        <v>254</v>
+      </c>
+      <c r="E76" t="s">
+        <v>257</v>
+      </c>
+      <c r="F76" t="s">
+        <v>105</v>
+      </c>
+      <c r="G76">
+        <v>2014</v>
+      </c>
+      <c r="H76">
+        <v>2014</v>
+      </c>
+      <c r="I76" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>261</v>
+      </c>
+      <c r="C77">
+        <v>2016</v>
+      </c>
+      <c r="D77" t="s">
+        <v>262</v>
+      </c>
+      <c r="E77" t="s">
+        <v>239</v>
+      </c>
+      <c r="F77" t="s">
+        <v>105</v>
+      </c>
+      <c r="G77">
+        <v>2016</v>
+      </c>
+      <c r="H77">
+        <v>2016</v>
+      </c>
+      <c r="I77" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>264</v>
+      </c>
+      <c r="C78">
+        <v>2016</v>
+      </c>
+      <c r="D78" t="s">
+        <v>262</v>
+      </c>
+      <c r="E78" t="s">
+        <v>265</v>
+      </c>
+      <c r="F78" t="s">
+        <v>105</v>
+      </c>
+      <c r="G78">
+        <v>2016</v>
+      </c>
+      <c r="H78">
+        <v>2016</v>
+      </c>
+      <c r="I78" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>267</v>
+      </c>
+      <c r="C79">
+        <v>2016</v>
+      </c>
+      <c r="D79" t="s">
+        <v>262</v>
+      </c>
+      <c r="E79" t="s">
+        <v>268</v>
+      </c>
+      <c r="F79" t="s">
+        <v>105</v>
+      </c>
+      <c r="G79">
+        <v>2016</v>
+      </c>
+      <c r="H79">
+        <v>2016</v>
+      </c>
+      <c r="I79" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>270</v>
+      </c>
+      <c r="C80">
+        <v>1952</v>
+      </c>
+      <c r="D80" t="s">
+        <v>216</v>
+      </c>
+      <c r="E80" t="s">
+        <v>271</v>
+      </c>
+      <c r="F80" t="s">
+        <v>105</v>
+      </c>
+      <c r="G80">
+        <v>1952</v>
+      </c>
+      <c r="H80">
+        <v>1952</v>
+      </c>
+      <c r="I80" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>273</v>
+      </c>
+      <c r="C81">
+        <v>1952</v>
+      </c>
+      <c r="D81" t="s">
+        <v>250</v>
+      </c>
+      <c r="E81" t="s">
+        <v>274</v>
+      </c>
+      <c r="F81" t="s">
+        <v>105</v>
+      </c>
+      <c r="G81">
+        <v>1952</v>
+      </c>
+      <c r="H81">
+        <v>1952</v>
+      </c>
+      <c r="I81" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>273</v>
+      </c>
+      <c r="C82">
+        <v>1952</v>
+      </c>
+      <c r="D82" t="s">
+        <v>250</v>
+      </c>
+      <c r="E82" t="s">
+        <v>277</v>
+      </c>
+      <c r="F82" t="s">
+        <v>105</v>
+      </c>
+      <c r="G82">
+        <v>1952</v>
+      </c>
+      <c r="H82">
+        <v>1952</v>
+      </c>
+      <c r="I82" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>278</v>
+      </c>
+      <c r="C83">
+        <v>1952</v>
+      </c>
+      <c r="D83" t="s">
+        <v>201</v>
+      </c>
+      <c r="E83" t="s">
+        <v>125</v>
+      </c>
+      <c r="F83" t="s">
+        <v>126</v>
+      </c>
+      <c r="G83">
+        <v>1952</v>
+      </c>
+      <c r="H83">
+        <v>1952</v>
+      </c>
+      <c r="I83" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>280</v>
+      </c>
+      <c r="C84">
+        <v>1952</v>
+      </c>
+      <c r="D84" t="s">
+        <v>216</v>
+      </c>
+      <c r="E84" t="s">
+        <v>281</v>
+      </c>
+      <c r="F84" t="s">
+        <v>126</v>
+      </c>
+      <c r="G84">
+        <v>1952</v>
+      </c>
+      <c r="H84">
+        <v>1952</v>
+      </c>
+      <c r="I84" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>283</v>
+      </c>
+      <c r="C85">
+        <v>1952</v>
+      </c>
+      <c r="D85" t="s">
+        <v>216</v>
+      </c>
+      <c r="E85" t="s">
+        <v>284</v>
+      </c>
+      <c r="F85" t="s">
+        <v>126</v>
+      </c>
+      <c r="G85">
+        <v>1952</v>
+      </c>
+      <c r="H85">
+        <v>1952</v>
+      </c>
+      <c r="I85" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>286</v>
+      </c>
+      <c r="C86">
+        <v>1952</v>
+      </c>
+      <c r="D86" t="s">
+        <v>250</v>
+      </c>
+      <c r="E86" t="s">
+        <v>287</v>
+      </c>
+      <c r="F86" t="s">
+        <v>126</v>
+      </c>
+      <c r="G86">
+        <v>1952</v>
+      </c>
+      <c r="H86">
+        <v>1952</v>
+      </c>
+      <c r="I86" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>289</v>
+      </c>
+      <c r="C87">
+        <v>1952</v>
+      </c>
+      <c r="D87" t="s">
+        <v>290</v>
+      </c>
+      <c r="E87" t="s">
+        <v>291</v>
+      </c>
+      <c r="F87" t="s">
+        <v>105</v>
+      </c>
+      <c r="G87">
+        <v>1952</v>
+      </c>
+      <c r="H87">
+        <v>1952</v>
+      </c>
+      <c r="I87" t="s">
+        <v>292</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed unused files, updated ELAN files, updated metadata
</commit_message>
<xml_diff>
--- a/corpus/evenki/current_meta.xlsx
+++ b/corpus/evenki/current_meta.xlsx
@@ -1319,11 +1319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1363,7 +1362,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1392,7 +1391,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1421,7 +1420,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1476,7 +1475,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1505,7 +1504,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1534,7 +1533,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1563,7 +1562,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1592,7 +1591,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1621,7 +1620,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1650,7 +1649,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1679,7 +1678,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1708,7 +1707,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1737,7 +1736,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1766,7 +1765,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1795,7 +1794,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1824,7 +1823,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1853,7 +1852,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1882,7 +1881,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1911,7 +1910,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1940,7 +1939,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1969,7 +1968,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1998,7 +1997,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2027,7 +2026,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2056,7 +2055,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2085,7 +2084,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2114,7 +2113,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2143,7 +2142,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2172,7 +2171,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2201,7 +2200,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2230,7 +2229,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2259,7 +2258,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2288,7 +2287,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2317,7 +2316,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2343,7 +2342,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2369,7 +2368,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2398,7 +2397,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2456,7 +2455,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2485,7 +2484,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2514,7 +2513,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2540,7 +2539,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2569,7 +2568,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2627,7 +2626,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2656,7 +2655,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2685,7 +2684,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2714,7 +2713,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2743,7 +2742,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2772,7 +2771,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2801,7 +2800,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2830,7 +2829,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2859,7 +2858,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2888,7 +2887,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2917,7 +2916,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2946,7 +2945,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1">
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2972,7 +2971,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1">
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -3001,7 +3000,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1">
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -3028,7 +3027,7 @@
       </c>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" hidden="1">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -3054,7 +3053,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1">
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -3080,7 +3079,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1">
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -3109,7 +3108,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1">
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -3138,7 +3137,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1">
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -3164,7 +3163,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1">
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -3198,7 +3197,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1">
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -3227,7 +3226,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1">
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -3253,7 +3252,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1">
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -3282,7 +3281,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1">
+    <row r="70" spans="1:9">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -3311,7 +3310,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1">
+    <row r="71" spans="1:9">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -3340,7 +3339,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="72" spans="1:9" hidden="1">
+    <row r="72" spans="1:9">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -3369,7 +3368,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1">
+    <row r="73" spans="1:9">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -3398,7 +3397,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="74" spans="1:9" hidden="1">
+    <row r="74" spans="1:9">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -3427,7 +3426,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="75" spans="1:9" hidden="1">
+    <row r="75" spans="1:9">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -3456,7 +3455,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1">
+    <row r="76" spans="1:9">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -3485,7 +3484,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="77" spans="1:9" hidden="1">
+    <row r="77" spans="1:9">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -3514,7 +3513,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1">
+    <row r="78" spans="1:9">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -3543,7 +3542,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1">
+    <row r="79" spans="1:9">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -3572,7 +3571,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="80" spans="1:9" hidden="1">
+    <row r="80" spans="1:9">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -3589,7 +3588,7 @@
         <v>271</v>
       </c>
       <c r="F80" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G80">
         <v>1952</v>
@@ -3601,7 +3600,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="81" spans="1:9" hidden="1">
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -3630,7 +3629,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1">
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -3659,7 +3658,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="83" spans="1:9" hidden="1">
+    <row r="83" spans="1:9">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -3688,7 +3687,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="84" spans="1:9" hidden="1">
+    <row r="84" spans="1:9">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -3717,7 +3716,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="85" spans="1:9" hidden="1">
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -3746,7 +3745,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="1:9" hidden="1">
+    <row r="86" spans="1:9">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -3775,7 +3774,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="87" spans="1:9" hidden="1">
+    <row r="87" spans="1:9">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -3806,9 +3805,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I87">
-    <filterColumn colId="1">
-      <filters blank="1"/>
-    </filterColumn>
+    <filterColumn colId="1"/>
   </autoFilter>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>

</xml_diff>

<commit_message>
added new files, fixed links in meta
</commit_message>
<xml_diff>
--- a/corpus/evenki/current_meta.xlsx
+++ b/corpus/evenki/current_meta.xlsx
@@ -10,8 +10,8 @@
     <sheet name="texts" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">texts!$A$1:$I$107</definedName>
-    <definedName name="meta" localSheetId="0">texts!$A$1:$A$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">texts!$A$1:$I$109</definedName>
+    <definedName name="meta" localSheetId="0">texts!$A$1:$A$109</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="375">
   <si>
     <t>filename</t>
   </si>
@@ -1134,6 +1134,27 @@
   </si>
   <si>
     <t>http://siberian-lang.srcc.msu.ru/ru/node/4889451</t>
+  </si>
+  <si>
+    <t>http://siberian-lang.srcc.msu.ru/node/4889445</t>
+  </si>
+  <si>
+    <t>2007_Mutoray_Yastrikova_FSk2_transliterated.eaf</t>
+  </si>
+  <si>
+    <t>2007_Mutoray_Yastrikova_FSk5_transliterated.eaf</t>
+  </si>
+  <si>
+    <t>Ястрикова Ирина Михайловна</t>
+  </si>
+  <si>
+    <t>http://siberian-lang.srcc.msu.ru/node/4889455</t>
+  </si>
+  <si>
+    <t>Беззубые</t>
+  </si>
+  <si>
+    <t>http://siberian-lang.srcc.msu.ru/ru/node/4889453/</t>
   </si>
 </sst>
 </file>
@@ -1520,10 +1541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2809,19 +2830,19 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>369</v>
       </c>
       <c r="B41" t="s">
-        <v>178</v>
+        <v>371</v>
       </c>
       <c r="C41">
         <v>2007</v>
       </c>
       <c r="D41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E41" t="s">
-        <v>295</v>
+        <v>125</v>
       </c>
       <c r="F41" t="s">
         <v>105</v>
@@ -2833,7 +2854,7 @@
         <v>2007</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>296</v>
+        <v>372</v>
       </c>
       <c r="J41" t="s">
         <v>358</v>
@@ -2841,19 +2862,19 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="B42" t="s">
-        <v>178</v>
+        <v>371</v>
       </c>
       <c r="C42">
         <v>2007</v>
       </c>
       <c r="D42" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E42" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="F42" t="s">
         <v>105</v>
@@ -2865,7 +2886,7 @@
         <v>2007</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="J42" t="s">
         <v>358</v>
@@ -2873,7 +2894,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>361</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
         <v>178</v>
@@ -2885,7 +2906,7 @@
         <v>179</v>
       </c>
       <c r="E43" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F43" t="s">
         <v>105</v>
@@ -2896,7 +2917,7 @@
       <c r="H43">
         <v>2007</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="I43" s="1" t="s">
         <v>296</v>
       </c>
       <c r="J43" t="s">
@@ -2905,7 +2926,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>365</v>
       </c>
       <c r="B44" t="s">
         <v>178</v>
@@ -2917,7 +2938,7 @@
         <v>179</v>
       </c>
       <c r="E44" t="s">
-        <v>182</v>
+        <v>366</v>
       </c>
       <c r="F44" t="s">
         <v>105</v>
@@ -2929,7 +2950,7 @@
         <v>2007</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>183</v>
+        <v>367</v>
       </c>
       <c r="J44" t="s">
         <v>358</v>
@@ -2937,7 +2958,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>361</v>
       </c>
       <c r="B45" t="s">
         <v>178</v>
@@ -2949,7 +2970,7 @@
         <v>179</v>
       </c>
       <c r="E45" t="s">
-        <v>180</v>
+        <v>294</v>
       </c>
       <c r="F45" t="s">
         <v>105</v>
@@ -2961,7 +2982,7 @@
         <v>2007</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>181</v>
+        <v>368</v>
       </c>
       <c r="J45" t="s">
         <v>358</v>
@@ -2969,10 +2990,10 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C46">
         <v>2007</v>
@@ -2981,7 +3002,7 @@
         <v>179</v>
       </c>
       <c r="E46" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F46" t="s">
         <v>105</v>
@@ -2993,18 +3014,18 @@
         <v>2007</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J46" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C47">
         <v>2007</v>
@@ -3013,7 +3034,7 @@
         <v>179</v>
       </c>
       <c r="E47" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="F47" t="s">
         <v>105</v>
@@ -3025,68 +3046,71 @@
         <v>2007</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="J47" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>297</v>
+        <v>184</v>
       </c>
       <c r="C48">
-        <v>2005</v>
+        <v>2007</v>
       </c>
       <c r="D48" t="s">
-        <v>298</v>
+        <v>179</v>
       </c>
       <c r="E48" t="s">
-        <v>299</v>
+        <v>185</v>
       </c>
       <c r="F48" t="s">
         <v>105</v>
       </c>
       <c r="G48">
-        <v>2005</v>
+        <v>2007</v>
       </c>
       <c r="H48">
-        <v>2005</v>
+        <v>2007</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="J48" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B49" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C49">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="D49" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="E49" t="s">
-        <v>98</v>
+        <v>187</v>
       </c>
       <c r="F49" t="s">
         <v>105</v>
       </c>
       <c r="G49">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="H49">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="J49" t="s">
         <v>359</v>
@@ -3094,42 +3118,39 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B50" t="s">
-        <v>192</v>
+        <v>297</v>
       </c>
       <c r="C50">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="D50" t="s">
-        <v>190</v>
+        <v>298</v>
       </c>
       <c r="E50" t="s">
-        <v>98</v>
+        <v>299</v>
       </c>
       <c r="F50" t="s">
         <v>105</v>
       </c>
       <c r="G50">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="H50">
-        <v>2008</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>193</v>
+        <v>2005</v>
       </c>
       <c r="J50" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B51" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C51">
         <v>2008</v>
@@ -3150,18 +3171,18 @@
         <v>2008</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="J51" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C52">
         <v>2008</v>
@@ -3170,7 +3191,7 @@
         <v>190</v>
       </c>
       <c r="E52" t="s">
-        <v>194</v>
+        <v>98</v>
       </c>
       <c r="F52" t="s">
         <v>105</v>
@@ -3182,15 +3203,15 @@
         <v>2008</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J52" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B53" t="s">
         <v>196</v>
@@ -3202,7 +3223,7 @@
         <v>190</v>
       </c>
       <c r="E53" t="s">
-        <v>198</v>
+        <v>98</v>
       </c>
       <c r="F53" t="s">
         <v>105</v>
@@ -3214,7 +3235,7 @@
         <v>2008</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J53" t="s">
         <v>358</v>
@@ -3222,7 +3243,7 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>325</v>
+        <v>45</v>
       </c>
       <c r="B54" t="s">
         <v>196</v>
@@ -3234,10 +3255,10 @@
         <v>190</v>
       </c>
       <c r="E54" t="s">
-        <v>326</v>
+        <v>194</v>
       </c>
       <c r="F54" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G54">
         <v>2008</v>
@@ -3246,7 +3267,7 @@
         <v>2008</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>327</v>
+        <v>195</v>
       </c>
       <c r="J54" t="s">
         <v>358</v>
@@ -3254,19 +3275,19 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B55" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C55">
         <v>2008</v>
       </c>
       <c r="D55" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="E55" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F55" t="s">
         <v>105</v>
@@ -3278,7 +3299,7 @@
         <v>2008</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="J55" t="s">
         <v>358</v>
@@ -3286,22 +3307,22 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>325</v>
       </c>
       <c r="B56" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C56">
         <v>2008</v>
       </c>
       <c r="D56" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="E56" t="s">
-        <v>204</v>
+        <v>326</v>
       </c>
       <c r="F56" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G56">
         <v>2008</v>
@@ -3310,7 +3331,7 @@
         <v>2008</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>205</v>
+        <v>327</v>
       </c>
       <c r="J56" t="s">
         <v>358</v>
@@ -3318,10 +3339,10 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>316</v>
+        <v>47</v>
       </c>
       <c r="B57" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C57">
         <v>2008</v>
@@ -3330,10 +3351,10 @@
         <v>201</v>
       </c>
       <c r="E57" t="s">
-        <v>317</v>
+        <v>202</v>
       </c>
       <c r="F57" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G57">
         <v>2008</v>
@@ -3341,19 +3362,19 @@
       <c r="H57">
         <v>2008</v>
       </c>
-      <c r="I57" s="4" t="s">
-        <v>318</v>
+      <c r="I57" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="J57" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>362</v>
+        <v>48</v>
       </c>
       <c r="B58" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C58">
         <v>2008</v>
@@ -3362,7 +3383,7 @@
         <v>201</v>
       </c>
       <c r="E58" t="s">
-        <v>320</v>
+        <v>204</v>
       </c>
       <c r="F58" t="s">
         <v>105</v>
@@ -3374,15 +3395,15 @@
         <v>2008</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>321</v>
+        <v>205</v>
       </c>
       <c r="J58" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>49</v>
+        <v>316</v>
       </c>
       <c r="B59" t="s">
         <v>206</v>
@@ -3394,7 +3415,7 @@
         <v>201</v>
       </c>
       <c r="E59" t="s">
-        <v>210</v>
+        <v>317</v>
       </c>
       <c r="F59" t="s">
         <v>126</v>
@@ -3405,8 +3426,8 @@
       <c r="H59">
         <v>2008</v>
       </c>
-      <c r="I59" s="1" t="s">
-        <v>211</v>
+      <c r="I59" s="4" t="s">
+        <v>318</v>
       </c>
       <c r="J59" t="s">
         <v>359</v>
@@ -3414,7 +3435,7 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>50</v>
+        <v>362</v>
       </c>
       <c r="B60" t="s">
         <v>206</v>
@@ -3426,10 +3447,10 @@
         <v>201</v>
       </c>
       <c r="E60" t="s">
-        <v>212</v>
+        <v>320</v>
       </c>
       <c r="F60" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G60">
         <v>2008</v>
@@ -3438,7 +3459,7 @@
         <v>2008</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>213</v>
+        <v>321</v>
       </c>
       <c r="J60" t="s">
         <v>359</v>
@@ -3446,7 +3467,7 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B61" t="s">
         <v>206</v>
@@ -3458,7 +3479,7 @@
         <v>201</v>
       </c>
       <c r="E61" t="s">
-        <v>319</v>
+        <v>210</v>
       </c>
       <c r="F61" t="s">
         <v>126</v>
@@ -3470,7 +3491,7 @@
         <v>2008</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J61" t="s">
         <v>359</v>
@@ -3478,7 +3499,7 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B62" t="s">
         <v>206</v>
@@ -3490,10 +3511,10 @@
         <v>201</v>
       </c>
       <c r="E62" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="F62" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G62">
         <v>2008</v>
@@ -3502,7 +3523,7 @@
         <v>2008</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="J62" t="s">
         <v>359</v>
@@ -3510,22 +3531,22 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B63" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C63">
         <v>2008</v>
       </c>
       <c r="D63" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="E63" t="s">
-        <v>216</v>
+        <v>319</v>
       </c>
       <c r="F63" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G63">
         <v>2008</v>
@@ -3534,27 +3555,27 @@
         <v>2008</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="J63" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B64" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C64">
         <v>2008</v>
       </c>
       <c r="D64" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="E64" t="s">
-        <v>98</v>
+        <v>207</v>
       </c>
       <c r="F64" t="s">
         <v>105</v>
@@ -3566,7 +3587,7 @@
         <v>2008</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="J64" t="s">
         <v>359</v>
@@ -3574,10 +3595,10 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B65" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C65">
         <v>2008</v>
@@ -3586,7 +3607,7 @@
         <v>215</v>
       </c>
       <c r="E65" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F65" t="s">
         <v>105</v>
@@ -3598,18 +3619,18 @@
         <v>2008</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J65" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B66" t="s">
-        <v>300</v>
+        <v>218</v>
       </c>
       <c r="C66">
         <v>2008</v>
@@ -3629,48 +3650,51 @@
       <c r="H66">
         <v>2008</v>
       </c>
+      <c r="I66" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="J66" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" s="6" customFormat="1">
-      <c r="A67" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="C67" s="6">
-        <v>2008</v>
-      </c>
-      <c r="D67" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" t="s">
+        <v>55</v>
+      </c>
+      <c r="B67" t="s">
+        <v>220</v>
+      </c>
+      <c r="C67">
+        <v>2008</v>
+      </c>
+      <c r="D67" t="s">
         <v>215</v>
       </c>
-      <c r="E67" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G67" s="6">
-        <v>2008</v>
-      </c>
-      <c r="H67" s="6">
-        <v>2008</v>
-      </c>
-      <c r="I67" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="J67" s="6" t="s">
-        <v>358</v>
+      <c r="E67" t="s">
+        <v>221</v>
+      </c>
+      <c r="F67" t="s">
+        <v>105</v>
+      </c>
+      <c r="G67">
+        <v>2008</v>
+      </c>
+      <c r="H67">
+        <v>2008</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J67" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>223</v>
+        <v>300</v>
       </c>
       <c r="C68">
         <v>2008</v>
@@ -3679,10 +3703,10 @@
         <v>215</v>
       </c>
       <c r="E68" t="s">
-        <v>224</v>
+        <v>98</v>
       </c>
       <c r="F68" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G68">
         <v>2008</v>
@@ -3690,49 +3714,48 @@
       <c r="H68">
         <v>2008</v>
       </c>
-      <c r="I68" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="J68" s="6" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
-      <c r="A69" t="s">
-        <v>58</v>
-      </c>
-      <c r="B69" t="s">
-        <v>301</v>
-      </c>
-      <c r="C69">
-        <v>2008</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="J68" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" s="6" customFormat="1">
+      <c r="A69" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C69" s="6">
+        <v>2008</v>
+      </c>
+      <c r="D69" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E69" t="s">
-        <v>98</v>
-      </c>
-      <c r="F69" t="s">
-        <v>105</v>
-      </c>
-      <c r="G69">
-        <v>2008</v>
-      </c>
-      <c r="H69">
-        <v>2008</v>
-      </c>
-      <c r="I69" s="1"/>
+      <c r="E69" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G69" s="6">
+        <v>2008</v>
+      </c>
+      <c r="H69" s="6">
+        <v>2008</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>324</v>
+      </c>
       <c r="J69" s="6" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B70" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
       <c r="C70">
         <v>2008</v>
@@ -3741,16 +3764,19 @@
         <v>215</v>
       </c>
       <c r="E70" t="s">
-        <v>98</v>
+        <v>224</v>
       </c>
       <c r="F70" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G70">
         <v>2008</v>
       </c>
       <c r="H70">
         <v>2008</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="J70" s="6" t="s">
         <v>358</v>
@@ -3758,7 +3784,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B71" t="s">
         <v>301</v>
@@ -3781,98 +3807,96 @@
       <c r="H71">
         <v>2008</v>
       </c>
+      <c r="I71" s="1"/>
       <c r="J71" s="6" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B72" t="s">
-        <v>226</v>
+        <v>301</v>
       </c>
       <c r="C72">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="D72" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="E72" t="s">
-        <v>228</v>
+        <v>98</v>
       </c>
       <c r="F72" t="s">
         <v>105</v>
       </c>
       <c r="G72">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="H72">
-        <v>2009</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>229</v>
+        <v>2008</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B73" t="s">
-        <v>226</v>
+        <v>301</v>
       </c>
       <c r="C73">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="D73" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="E73" t="s">
-        <v>230</v>
+        <v>98</v>
       </c>
       <c r="F73" t="s">
         <v>105</v>
       </c>
       <c r="G73">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="H73">
-        <v>2009</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>231</v>
+        <v>2008</v>
       </c>
       <c r="J73" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B74" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C74">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="D74" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E74" t="s">
-        <v>302</v>
+        <v>228</v>
       </c>
       <c r="F74" t="s">
         <v>105</v>
       </c>
       <c r="G74">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="H74">
-        <v>2010</v>
+        <v>2009</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="J74" s="6" t="s">
         <v>359</v>
@@ -3880,31 +3904,31 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B75" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C75">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="D75" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E75" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F75" t="s">
         <v>105</v>
       </c>
       <c r="G75">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="H75">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="J75" s="6" t="s">
         <v>359</v>
@@ -3912,71 +3936,68 @@
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="B76" t="s">
+        <v>232</v>
+      </c>
+      <c r="C76">
+        <v>2010</v>
+      </c>
+      <c r="D76" t="s">
+        <v>233</v>
+      </c>
+      <c r="E76" t="s">
+        <v>302</v>
+      </c>
+      <c r="F76" t="s">
+        <v>105</v>
+      </c>
+      <c r="G76">
+        <v>2010</v>
+      </c>
+      <c r="H76">
+        <v>2010</v>
       </c>
       <c r="J76" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>328</v>
+        <v>64</v>
       </c>
       <c r="B77" t="s">
-        <v>303</v>
+        <v>232</v>
       </c>
       <c r="C77">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="D77" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E77" t="s">
-        <v>329</v>
+        <v>234</v>
       </c>
       <c r="F77" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G77">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="H77">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>330</v>
+        <v>235</v>
       </c>
       <c r="J77" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>66</v>
-      </c>
-      <c r="B78" t="s">
-        <v>303</v>
-      </c>
-      <c r="C78">
-        <v>2011</v>
-      </c>
-      <c r="D78" t="s">
-        <v>236</v>
-      </c>
-      <c r="E78" t="s">
-        <v>98</v>
-      </c>
-      <c r="F78" t="s">
-        <v>105</v>
-      </c>
-      <c r="G78">
-        <v>2011</v>
-      </c>
-      <c r="H78">
-        <v>2011</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>304</v>
+        <v>65</v>
       </c>
       <c r="J78" s="6" t="s">
         <v>358</v>
@@ -3984,7 +4005,7 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>67</v>
+        <v>328</v>
       </c>
       <c r="B79" t="s">
         <v>303</v>
@@ -3996,10 +4017,10 @@
         <v>236</v>
       </c>
       <c r="E79" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="F79" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G79">
         <v>2011</v>
@@ -4007,16 +4028,19 @@
       <c r="H79">
         <v>2011</v>
       </c>
+      <c r="I79" s="1" t="s">
+        <v>330</v>
+      </c>
       <c r="J79" s="6" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B80" t="s">
-        <v>237</v>
+        <v>303</v>
       </c>
       <c r="C80">
         <v>2011</v>
@@ -4025,7 +4049,7 @@
         <v>236</v>
       </c>
       <c r="E80" t="s">
-        <v>238</v>
+        <v>98</v>
       </c>
       <c r="F80" t="s">
         <v>105</v>
@@ -4037,7 +4061,7 @@
         <v>2011</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>239</v>
+        <v>304</v>
       </c>
       <c r="J80" s="6" t="s">
         <v>358</v>
@@ -4045,10 +4069,10 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B81" t="s">
-        <v>237</v>
+        <v>303</v>
       </c>
       <c r="C81">
         <v>2011</v>
@@ -4057,7 +4081,7 @@
         <v>236</v>
       </c>
       <c r="E81" t="s">
-        <v>98</v>
+        <v>305</v>
       </c>
       <c r="F81" t="s">
         <v>105</v>
@@ -4068,16 +4092,13 @@
       <c r="H81">
         <v>2011</v>
       </c>
-      <c r="I81" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="J81" s="6" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>331</v>
+        <v>68</v>
       </c>
       <c r="B82" t="s">
         <v>237</v>
@@ -4089,10 +4110,10 @@
         <v>236</v>
       </c>
       <c r="E82" t="s">
-        <v>283</v>
+        <v>238</v>
       </c>
       <c r="F82" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G82">
         <v>2011</v>
@@ -4101,7 +4122,7 @@
         <v>2011</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>332</v>
+        <v>239</v>
       </c>
       <c r="J82" s="6" t="s">
         <v>358</v>
@@ -4109,7 +4130,7 @@
     </row>
     <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>333</v>
+        <v>69</v>
       </c>
       <c r="B83" t="s">
         <v>237</v>
@@ -4121,10 +4142,10 @@
         <v>236</v>
       </c>
       <c r="E83" t="s">
-        <v>334</v>
+        <v>98</v>
       </c>
       <c r="F83" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G83">
         <v>2011</v>
@@ -4133,7 +4154,7 @@
         <v>2011</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>335</v>
+        <v>240</v>
       </c>
       <c r="J83" s="6" t="s">
         <v>358</v>
@@ -4141,19 +4162,19 @@
     </row>
     <row r="84" spans="1:10">
       <c r="A84" t="s">
-        <v>70</v>
+        <v>331</v>
       </c>
       <c r="B84" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C84">
         <v>2011</v>
       </c>
       <c r="D84" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E84" t="s">
-        <v>243</v>
+        <v>283</v>
       </c>
       <c r="F84" t="s">
         <v>126</v>
@@ -4165,7 +4186,7 @@
         <v>2011</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>244</v>
+        <v>332</v>
       </c>
       <c r="J84" s="6" t="s">
         <v>358</v>
@@ -4173,19 +4194,19 @@
     </row>
     <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B85" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C85">
         <v>2011</v>
       </c>
       <c r="D85" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E85" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F85" t="s">
         <v>126</v>
@@ -4196,8 +4217,8 @@
       <c r="H85">
         <v>2011</v>
       </c>
-      <c r="I85" s="4" t="s">
-        <v>338</v>
+      <c r="I85" s="1" t="s">
+        <v>335</v>
       </c>
       <c r="J85" s="6" t="s">
         <v>358</v>
@@ -4205,31 +4226,31 @@
     </row>
     <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B86" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C86">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="D86" t="s">
-        <v>201</v>
+        <v>242</v>
       </c>
       <c r="E86" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F86" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G86">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="H86">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="J86" s="6" t="s">
         <v>358</v>
@@ -4237,31 +4258,31 @@
     </row>
     <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>72</v>
+        <v>336</v>
       </c>
       <c r="B87" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C87">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="D87" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="E87" t="s">
-        <v>250</v>
+        <v>337</v>
       </c>
       <c r="F87" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G87">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="H87">
-        <v>2014</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>251</v>
+        <v>2011</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>338</v>
       </c>
       <c r="J87" s="6" t="s">
         <v>358</v>
@@ -4269,19 +4290,19 @@
     </row>
     <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>339</v>
+        <v>71</v>
       </c>
       <c r="B88" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C88">
         <v>2014</v>
       </c>
       <c r="D88" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
       <c r="E88" t="s">
-        <v>340</v>
+        <v>246</v>
       </c>
       <c r="F88" t="s">
         <v>105</v>
@@ -4293,7 +4314,7 @@
         <v>2014</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>341</v>
+        <v>247</v>
       </c>
       <c r="J88" s="6" t="s">
         <v>358</v>
@@ -4301,22 +4322,22 @@
     </row>
     <row r="89" spans="1:10">
       <c r="A89" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B89" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C89">
         <v>2014</v>
       </c>
       <c r="D89" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E89" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F89" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G89">
         <v>2014</v>
@@ -4325,27 +4346,27 @@
         <v>2014</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="J89" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" t="s">
-        <v>74</v>
+        <v>339</v>
       </c>
       <c r="B90" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C90">
         <v>2014</v>
       </c>
       <c r="D90" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E90" t="s">
-        <v>258</v>
+        <v>340</v>
       </c>
       <c r="F90" t="s">
         <v>105</v>
@@ -4357,15 +4378,15 @@
         <v>2014</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>259</v>
+        <v>341</v>
       </c>
       <c r="J90" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B91" t="s">
         <v>252</v>
@@ -4377,10 +4398,10 @@
         <v>253</v>
       </c>
       <c r="E91" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F91" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G91">
         <v>2014</v>
@@ -4389,7 +4410,7 @@
         <v>2014</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J91" s="6" t="s">
         <v>359</v>
@@ -4397,7 +4418,7 @@
     </row>
     <row r="92" spans="1:10">
       <c r="A92" t="s">
-        <v>342</v>
+        <v>74</v>
       </c>
       <c r="B92" t="s">
         <v>252</v>
@@ -4409,10 +4430,10 @@
         <v>253</v>
       </c>
       <c r="E92" t="s">
-        <v>343</v>
+        <v>258</v>
       </c>
       <c r="F92" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G92">
         <v>2014</v>
@@ -4421,7 +4442,7 @@
         <v>2014</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>344</v>
+        <v>259</v>
       </c>
       <c r="J92" s="6" t="s">
         <v>359</v>
@@ -4429,63 +4450,63 @@
     </row>
     <row r="93" spans="1:10">
       <c r="A93" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B93" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C93">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="D93" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="E93" t="s">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="F93" t="s">
         <v>105</v>
       </c>
       <c r="G93">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="H93">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="J93" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B94" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="C94">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="D94" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="E94" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="F94" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G94">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="H94">
-        <v>2016</v>
-      </c>
-      <c r="I94" s="4" t="s">
-        <v>347</v>
+        <v>2014</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>344</v>
       </c>
       <c r="J94" s="6" t="s">
         <v>359</v>
@@ -4493,10 +4514,10 @@
     </row>
     <row r="95" spans="1:10">
       <c r="A95" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B95" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C95">
         <v>2016</v>
@@ -4505,7 +4526,7 @@
         <v>261</v>
       </c>
       <c r="E95" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="F95" t="s">
         <v>105</v>
@@ -4517,18 +4538,18 @@
         <v>2016</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="J95" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" t="s">
-        <v>78</v>
+        <v>345</v>
       </c>
       <c r="B96" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C96">
         <v>2016</v>
@@ -4537,7 +4558,7 @@
         <v>261</v>
       </c>
       <c r="E96" t="s">
-        <v>267</v>
+        <v>346</v>
       </c>
       <c r="F96" t="s">
         <v>105</v>
@@ -4548,19 +4569,19 @@
       <c r="H96">
         <v>2016</v>
       </c>
-      <c r="I96" s="1" t="s">
-        <v>268</v>
+      <c r="I96" s="4" t="s">
+        <v>347</v>
       </c>
       <c r="J96" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" t="s">
-        <v>363</v>
+        <v>77</v>
       </c>
       <c r="B97" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C97">
         <v>2016</v>
@@ -4569,7 +4590,7 @@
         <v>261</v>
       </c>
       <c r="E97" t="s">
-        <v>320</v>
+        <v>264</v>
       </c>
       <c r="F97" t="s">
         <v>105</v>
@@ -4580,16 +4601,16 @@
       <c r="H97">
         <v>2016</v>
       </c>
-      <c r="I97" s="4" t="s">
-        <v>348</v>
+      <c r="I97" s="1" t="s">
+        <v>265</v>
       </c>
       <c r="J97" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" t="s">
-        <v>349</v>
+        <v>78</v>
       </c>
       <c r="B98" t="s">
         <v>266</v>
@@ -4601,10 +4622,10 @@
         <v>261</v>
       </c>
       <c r="E98" t="s">
-        <v>350</v>
+        <v>267</v>
       </c>
       <c r="F98" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G98">
         <v>2016</v>
@@ -4613,7 +4634,7 @@
         <v>2016</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>351</v>
+        <v>268</v>
       </c>
       <c r="J98" s="6" t="s">
         <v>358</v>
@@ -4621,19 +4642,19 @@
     </row>
     <row r="99" spans="1:10">
       <c r="A99" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
       <c r="B99" t="s">
-        <v>353</v>
+        <v>266</v>
       </c>
       <c r="C99">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="D99" t="s">
-        <v>354</v>
+        <v>261</v>
       </c>
       <c r="E99" t="s">
-        <v>355</v>
+        <v>320</v>
       </c>
       <c r="F99" t="s">
         <v>105</v>
@@ -4645,39 +4666,39 @@
         <v>2016</v>
       </c>
       <c r="I99" s="4" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="J99" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" t="s">
-        <v>79</v>
+        <v>349</v>
       </c>
       <c r="B100" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C100">
-        <v>1952</v>
+        <v>2016</v>
       </c>
       <c r="D100" t="s">
-        <v>215</v>
+        <v>261</v>
       </c>
       <c r="E100" t="s">
-        <v>270</v>
+        <v>350</v>
       </c>
       <c r="F100" t="s">
         <v>126</v>
       </c>
       <c r="G100">
-        <v>1952</v>
+        <v>2016</v>
       </c>
       <c r="H100">
-        <v>1952</v>
+        <v>2016</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>271</v>
+        <v>351</v>
       </c>
       <c r="J100" s="6" t="s">
         <v>358</v>
@@ -4685,31 +4706,31 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" t="s">
-        <v>80</v>
+        <v>352</v>
       </c>
       <c r="B101" t="s">
-        <v>272</v>
+        <v>353</v>
       </c>
       <c r="C101">
-        <v>1952</v>
+        <v>2018</v>
       </c>
       <c r="D101" t="s">
-        <v>249</v>
+        <v>354</v>
       </c>
       <c r="E101" t="s">
-        <v>273</v>
+        <v>355</v>
       </c>
       <c r="F101" t="s">
         <v>105</v>
       </c>
       <c r="G101">
-        <v>1952</v>
+        <v>2016</v>
       </c>
       <c r="H101">
-        <v>1952</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>275</v>
+        <v>2016</v>
+      </c>
+      <c r="I101" s="4" t="s">
+        <v>356</v>
       </c>
       <c r="J101" s="6" t="s">
         <v>359</v>
@@ -4717,22 +4738,22 @@
     </row>
     <row r="102" spans="1:10">
       <c r="A102" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B102" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C102">
         <v>1952</v>
       </c>
       <c r="D102" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="E102" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="F102" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G102">
         <v>1952</v>
@@ -4741,30 +4762,30 @@
         <v>1952</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="J102" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B103" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C103">
         <v>1952</v>
       </c>
       <c r="D103" t="s">
-        <v>201</v>
+        <v>249</v>
       </c>
       <c r="E103" t="s">
-        <v>125</v>
+        <v>273</v>
       </c>
       <c r="F103" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G103">
         <v>1952</v>
@@ -4773,30 +4794,30 @@
         <v>1952</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="J103" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="104" spans="1:10">
       <c r="A104" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B104" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C104">
         <v>1952</v>
       </c>
       <c r="D104" t="s">
-        <v>215</v>
+        <v>249</v>
       </c>
       <c r="E104" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F104" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G104">
         <v>1952</v>
@@ -4805,27 +4826,27 @@
         <v>1952</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="J104" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B105" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C105">
         <v>1952</v>
       </c>
       <c r="D105" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="E105" t="s">
-        <v>283</v>
+        <v>125</v>
       </c>
       <c r="F105" t="s">
         <v>126</v>
@@ -4837,7 +4858,7 @@
         <v>1952</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="J105" s="6" t="s">
         <v>358</v>
@@ -4845,19 +4866,19 @@
     </row>
     <row r="106" spans="1:10">
       <c r="A106" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B106" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C106">
         <v>1952</v>
       </c>
       <c r="D106" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="E106" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="F106" t="s">
         <v>126</v>
@@ -4869,7 +4890,7 @@
         <v>1952</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="J106" s="6" t="s">
         <v>358</v>
@@ -4877,22 +4898,22 @@
     </row>
     <row r="107" spans="1:10">
       <c r="A107" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B107" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C107">
         <v>1952</v>
       </c>
       <c r="D107" t="s">
-        <v>289</v>
+        <v>215</v>
       </c>
       <c r="E107" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F107" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G107">
         <v>1952</v>
@@ -4901,14 +4922,78 @@
         <v>1952</v>
       </c>
       <c r="I107" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="J107" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108" t="s">
+        <v>85</v>
+      </c>
+      <c r="B108" t="s">
+        <v>285</v>
+      </c>
+      <c r="C108">
+        <v>1952</v>
+      </c>
+      <c r="D108" t="s">
+        <v>249</v>
+      </c>
+      <c r="E108" t="s">
+        <v>286</v>
+      </c>
+      <c r="F108" t="s">
+        <v>126</v>
+      </c>
+      <c r="G108">
+        <v>1952</v>
+      </c>
+      <c r="H108">
+        <v>1952</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="J108" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" t="s">
+        <v>86</v>
+      </c>
+      <c r="B109" t="s">
+        <v>288</v>
+      </c>
+      <c r="C109">
+        <v>1952</v>
+      </c>
+      <c r="D109" t="s">
+        <v>289</v>
+      </c>
+      <c r="E109" t="s">
+        <v>290</v>
+      </c>
+      <c r="F109" t="s">
+        <v>105</v>
+      </c>
+      <c r="G109">
+        <v>1952</v>
+      </c>
+      <c r="H109">
+        <v>1952</v>
+      </c>
+      <c r="I109" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="J107" s="6" t="s">
+      <c r="J109" s="6" t="s">
         <v>359</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I107">
+  <autoFilter ref="A1:I109">
     <filterColumn colId="1"/>
   </autoFilter>
   <hyperlinks>
@@ -4944,62 +5029,65 @@
     <hyperlink ref="I35" r:id="rId30"/>
     <hyperlink ref="I36" r:id="rId31"/>
     <hyperlink ref="I38" r:id="rId32"/>
-    <hyperlink ref="I45" r:id="rId33"/>
-    <hyperlink ref="I44" r:id="rId34"/>
-    <hyperlink ref="I46" r:id="rId35"/>
-    <hyperlink ref="I47" r:id="rId36"/>
-    <hyperlink ref="I49" r:id="rId37"/>
-    <hyperlink ref="I50" r:id="rId38"/>
-    <hyperlink ref="I52" r:id="rId39"/>
-    <hyperlink ref="I51" r:id="rId40"/>
-    <hyperlink ref="I53" r:id="rId41"/>
-    <hyperlink ref="I55" r:id="rId42"/>
-    <hyperlink ref="I56" r:id="rId43"/>
-    <hyperlink ref="I62" r:id="rId44"/>
-    <hyperlink ref="I61" r:id="rId45"/>
-    <hyperlink ref="I59" r:id="rId46"/>
-    <hyperlink ref="I60" r:id="rId47"/>
-    <hyperlink ref="I63" r:id="rId48"/>
-    <hyperlink ref="I64" r:id="rId49"/>
-    <hyperlink ref="I65" r:id="rId50"/>
-    <hyperlink ref="I68" r:id="rId51"/>
-    <hyperlink ref="I72" r:id="rId52"/>
-    <hyperlink ref="I73" r:id="rId53"/>
-    <hyperlink ref="I75" r:id="rId54"/>
-    <hyperlink ref="I80" r:id="rId55"/>
-    <hyperlink ref="I81" r:id="rId56"/>
-    <hyperlink ref="I84" r:id="rId57"/>
-    <hyperlink ref="I86" r:id="rId58"/>
-    <hyperlink ref="I87" r:id="rId59"/>
-    <hyperlink ref="I89" r:id="rId60"/>
-    <hyperlink ref="I91" r:id="rId61"/>
-    <hyperlink ref="I90" r:id="rId62"/>
-    <hyperlink ref="I93" r:id="rId63"/>
-    <hyperlink ref="I95" r:id="rId64"/>
-    <hyperlink ref="I96" r:id="rId65"/>
-    <hyperlink ref="I100" r:id="rId66"/>
-    <hyperlink ref="I102" r:id="rId67"/>
-    <hyperlink ref="I101" r:id="rId68"/>
-    <hyperlink ref="I103" r:id="rId69"/>
-    <hyperlink ref="I104" r:id="rId70"/>
-    <hyperlink ref="I105" r:id="rId71"/>
-    <hyperlink ref="I106" r:id="rId72"/>
-    <hyperlink ref="I107" r:id="rId73"/>
-    <hyperlink ref="I41" r:id="rId74"/>
-    <hyperlink ref="I78" r:id="rId75"/>
+    <hyperlink ref="I47" r:id="rId33"/>
+    <hyperlink ref="I46" r:id="rId34"/>
+    <hyperlink ref="I48" r:id="rId35"/>
+    <hyperlink ref="I49" r:id="rId36"/>
+    <hyperlink ref="I51" r:id="rId37"/>
+    <hyperlink ref="I52" r:id="rId38"/>
+    <hyperlink ref="I54" r:id="rId39"/>
+    <hyperlink ref="I53" r:id="rId40"/>
+    <hyperlink ref="I55" r:id="rId41"/>
+    <hyperlink ref="I57" r:id="rId42"/>
+    <hyperlink ref="I58" r:id="rId43"/>
+    <hyperlink ref="I64" r:id="rId44"/>
+    <hyperlink ref="I63" r:id="rId45"/>
+    <hyperlink ref="I61" r:id="rId46"/>
+    <hyperlink ref="I62" r:id="rId47"/>
+    <hyperlink ref="I65" r:id="rId48"/>
+    <hyperlink ref="I66" r:id="rId49"/>
+    <hyperlink ref="I67" r:id="rId50"/>
+    <hyperlink ref="I70" r:id="rId51"/>
+    <hyperlink ref="I74" r:id="rId52"/>
+    <hyperlink ref="I75" r:id="rId53"/>
+    <hyperlink ref="I77" r:id="rId54"/>
+    <hyperlink ref="I82" r:id="rId55"/>
+    <hyperlink ref="I83" r:id="rId56"/>
+    <hyperlink ref="I86" r:id="rId57"/>
+    <hyperlink ref="I88" r:id="rId58"/>
+    <hyperlink ref="I89" r:id="rId59"/>
+    <hyperlink ref="I91" r:id="rId60"/>
+    <hyperlink ref="I93" r:id="rId61"/>
+    <hyperlink ref="I92" r:id="rId62"/>
+    <hyperlink ref="I95" r:id="rId63"/>
+    <hyperlink ref="I97" r:id="rId64"/>
+    <hyperlink ref="I98" r:id="rId65"/>
+    <hyperlink ref="I102" r:id="rId66"/>
+    <hyperlink ref="I104" r:id="rId67"/>
+    <hyperlink ref="I103" r:id="rId68"/>
+    <hyperlink ref="I105" r:id="rId69"/>
+    <hyperlink ref="I106" r:id="rId70"/>
+    <hyperlink ref="I107" r:id="rId71"/>
+    <hyperlink ref="I108" r:id="rId72"/>
+    <hyperlink ref="I109" r:id="rId73"/>
+    <hyperlink ref="I43" r:id="rId74"/>
+    <hyperlink ref="I80" r:id="rId75"/>
     <hyperlink ref="I4" r:id="rId76"/>
     <hyperlink ref="I24" r:id="rId77"/>
-    <hyperlink ref="I58" r:id="rId78"/>
-    <hyperlink ref="I54" r:id="rId79"/>
-    <hyperlink ref="I77" r:id="rId80"/>
-    <hyperlink ref="I82" r:id="rId81"/>
-    <hyperlink ref="I83" r:id="rId82"/>
-    <hyperlink ref="I88" r:id="rId83"/>
-    <hyperlink ref="I92" r:id="rId84"/>
-    <hyperlink ref="I98" r:id="rId85"/>
-    <hyperlink ref="I42" r:id="rId86"/>
+    <hyperlink ref="I60" r:id="rId78"/>
+    <hyperlink ref="I56" r:id="rId79"/>
+    <hyperlink ref="I79" r:id="rId80"/>
+    <hyperlink ref="I84" r:id="rId81"/>
+    <hyperlink ref="I85" r:id="rId82"/>
+    <hyperlink ref="I90" r:id="rId83"/>
+    <hyperlink ref="I94" r:id="rId84"/>
+    <hyperlink ref="I100" r:id="rId85"/>
+    <hyperlink ref="I44" r:id="rId86"/>
+    <hyperlink ref="I45" r:id="rId87"/>
+    <hyperlink ref="I41" r:id="rId88"/>
+    <hyperlink ref="I42" r:id="rId89"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId87"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId90"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new texts, fixed audio links
</commit_message>
<xml_diff>
--- a/corpus/evenki/current_meta.xlsx
+++ b/corpus/evenki/current_meta.xlsx
@@ -10,8 +10,8 @@
     <sheet name="texts" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">texts!$A$1:$I$110</definedName>
-    <definedName name="meta" localSheetId="0">texts!$A$1:$A$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">texts!$A$1:$I$111</definedName>
+    <definedName name="meta" localSheetId="0">texts!$A$1:$A$111</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="379">
   <si>
     <t>filename</t>
   </si>
@@ -1553,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69:H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3734,11 +3734,8 @@
       </c>
     </row>
     <row r="69" spans="1:10">
-      <c r="A69" t="s">
-        <v>56</v>
-      </c>
       <c r="B69" t="s">
-        <v>299</v>
+        <v>219</v>
       </c>
       <c r="C69">
         <v>2008</v>
@@ -3746,81 +3743,73 @@
       <c r="D69" t="s">
         <v>214</v>
       </c>
-      <c r="E69" t="s">
+      <c r="F69" t="s">
+        <v>105</v>
+      </c>
+      <c r="G69">
+        <v>2008</v>
+      </c>
+      <c r="H69">
+        <v>2008</v>
+      </c>
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" t="s">
+        <v>56</v>
+      </c>
+      <c r="B70" t="s">
+        <v>299</v>
+      </c>
+      <c r="C70">
+        <v>2008</v>
+      </c>
+      <c r="D70" t="s">
+        <v>214</v>
+      </c>
+      <c r="E70" t="s">
         <v>98</v>
       </c>
-      <c r="F69" t="s">
-        <v>105</v>
-      </c>
-      <c r="G69">
-        <v>2008</v>
-      </c>
-      <c r="H69">
-        <v>2008</v>
-      </c>
-      <c r="J69" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" s="6" customFormat="1">
-      <c r="A70" s="6" t="s">
+      <c r="F70" t="s">
+        <v>105</v>
+      </c>
+      <c r="G70">
+        <v>2008</v>
+      </c>
+      <c r="H70">
+        <v>2008</v>
+      </c>
+      <c r="J70" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" s="6" customFormat="1">
+      <c r="A71" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B71" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="C70" s="6">
-        <v>2008</v>
-      </c>
-      <c r="D70" s="6" t="s">
+      <c r="C71" s="6">
+        <v>2008</v>
+      </c>
+      <c r="D71" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="E70" s="6" t="s">
+      <c r="E71" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F70" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G70" s="6">
-        <v>2008</v>
-      </c>
-      <c r="H70" s="6">
-        <v>2008</v>
-      </c>
-      <c r="I70" s="7" t="s">
+      <c r="F71" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G71" s="6">
+        <v>2008</v>
+      </c>
+      <c r="H71" s="6">
+        <v>2008</v>
+      </c>
+      <c r="I71" s="7" t="s">
         <v>323</v>
-      </c>
-      <c r="J70" s="6" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="A71" t="s">
-        <v>57</v>
-      </c>
-      <c r="B71" t="s">
-        <v>222</v>
-      </c>
-      <c r="C71">
-        <v>2008</v>
-      </c>
-      <c r="D71" t="s">
-        <v>214</v>
-      </c>
-      <c r="E71" t="s">
-        <v>223</v>
-      </c>
-      <c r="F71" t="s">
-        <v>126</v>
-      </c>
-      <c r="G71">
-        <v>2008</v>
-      </c>
-      <c r="H71">
-        <v>2008</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="J71" s="6" t="s">
         <v>357</v>
@@ -3828,10 +3817,10 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B72" t="s">
-        <v>300</v>
+        <v>222</v>
       </c>
       <c r="C72">
         <v>2008</v>
@@ -3840,10 +3829,10 @@
         <v>214</v>
       </c>
       <c r="E72" t="s">
-        <v>98</v>
+        <v>223</v>
       </c>
       <c r="F72" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G72">
         <v>2008</v>
@@ -3851,14 +3840,16 @@
       <c r="H72">
         <v>2008</v>
       </c>
-      <c r="I72" s="1"/>
+      <c r="I72" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="J72" s="6" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B73" t="s">
         <v>300</v>
@@ -3881,13 +3872,14 @@
       <c r="H73">
         <v>2008</v>
       </c>
+      <c r="I73" s="1"/>
       <c r="J73" s="6" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B74" t="s">
         <v>300</v>
@@ -3916,39 +3908,36 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B75" t="s">
-        <v>225</v>
+        <v>300</v>
       </c>
       <c r="C75">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="D75" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="E75" t="s">
-        <v>227</v>
+        <v>98</v>
       </c>
       <c r="F75" t="s">
         <v>105</v>
       </c>
       <c r="G75">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="H75">
-        <v>2009</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>228</v>
+        <v>2008</v>
       </c>
       <c r="J75" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B76" t="s">
         <v>225</v>
@@ -3960,7 +3949,7 @@
         <v>226</v>
       </c>
       <c r="E76" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F76" t="s">
         <v>105</v>
@@ -3972,7 +3961,7 @@
         <v>2009</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J76" s="6" t="s">
         <v>358</v>
@@ -3980,28 +3969,31 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B77" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C77">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="D77" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E77" t="s">
-        <v>301</v>
+        <v>229</v>
       </c>
       <c r="F77" t="s">
         <v>105</v>
       </c>
       <c r="G77">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="H77">
-        <v>2010</v>
+        <v>2009</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="J77" s="6" t="s">
         <v>358</v>
@@ -4009,7 +4001,7 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B78" t="s">
         <v>231</v>
@@ -4021,7 +4013,7 @@
         <v>232</v>
       </c>
       <c r="E78" t="s">
-        <v>233</v>
+        <v>301</v>
       </c>
       <c r="F78" t="s">
         <v>105</v>
@@ -4032,48 +4024,45 @@
       <c r="H78">
         <v>2010</v>
       </c>
-      <c r="I78" s="1" t="s">
-        <v>234</v>
-      </c>
       <c r="J78" s="6" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="B79" t="s">
+        <v>231</v>
+      </c>
+      <c r="C79">
+        <v>2010</v>
+      </c>
+      <c r="D79" t="s">
+        <v>232</v>
+      </c>
+      <c r="E79" t="s">
+        <v>233</v>
+      </c>
+      <c r="F79" t="s">
+        <v>105</v>
+      </c>
+      <c r="G79">
+        <v>2010</v>
+      </c>
+      <c r="H79">
+        <v>2010</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="J79" s="6" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>327</v>
-      </c>
-      <c r="B80" t="s">
-        <v>302</v>
-      </c>
-      <c r="C80">
-        <v>2011</v>
-      </c>
-      <c r="D80" t="s">
-        <v>235</v>
-      </c>
-      <c r="E80" t="s">
-        <v>328</v>
-      </c>
-      <c r="F80" t="s">
-        <v>126</v>
-      </c>
-      <c r="G80">
-        <v>2011</v>
-      </c>
-      <c r="H80">
-        <v>2011</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>329</v>
+        <v>65</v>
       </c>
       <c r="J80" s="6" t="s">
         <v>357</v>
@@ -4081,7 +4070,7 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>66</v>
+        <v>327</v>
       </c>
       <c r="B81" t="s">
         <v>302</v>
@@ -4093,10 +4082,10 @@
         <v>235</v>
       </c>
       <c r="E81" t="s">
-        <v>98</v>
+        <v>328</v>
       </c>
       <c r="F81" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G81">
         <v>2011</v>
@@ -4105,7 +4094,7 @@
         <v>2011</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>303</v>
+        <v>329</v>
       </c>
       <c r="J81" s="6" t="s">
         <v>357</v>
@@ -4113,7 +4102,7 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B82" t="s">
         <v>302</v>
@@ -4125,7 +4114,7 @@
         <v>235</v>
       </c>
       <c r="E82" t="s">
-        <v>304</v>
+        <v>98</v>
       </c>
       <c r="F82" t="s">
         <v>105</v>
@@ -4136,16 +4125,19 @@
       <c r="H82">
         <v>2011</v>
       </c>
+      <c r="I82" s="1" t="s">
+        <v>303</v>
+      </c>
       <c r="J82" s="6" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B83" t="s">
-        <v>236</v>
+        <v>302</v>
       </c>
       <c r="C83">
         <v>2011</v>
@@ -4154,7 +4146,7 @@
         <v>235</v>
       </c>
       <c r="E83" t="s">
-        <v>237</v>
+        <v>304</v>
       </c>
       <c r="F83" t="s">
         <v>105</v>
@@ -4165,16 +4157,13 @@
       <c r="H83">
         <v>2011</v>
       </c>
-      <c r="I83" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="J83" s="6" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B84" t="s">
         <v>236</v>
@@ -4186,7 +4175,7 @@
         <v>235</v>
       </c>
       <c r="E84" t="s">
-        <v>98</v>
+        <v>237</v>
       </c>
       <c r="F84" t="s">
         <v>105</v>
@@ -4198,7 +4187,7 @@
         <v>2011</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J84" s="6" t="s">
         <v>357</v>
@@ -4206,7 +4195,7 @@
     </row>
     <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>330</v>
+        <v>69</v>
       </c>
       <c r="B85" t="s">
         <v>236</v>
@@ -4218,10 +4207,10 @@
         <v>235</v>
       </c>
       <c r="E85" t="s">
-        <v>282</v>
+        <v>98</v>
       </c>
       <c r="F85" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G85">
         <v>2011</v>
@@ -4230,7 +4219,7 @@
         <v>2011</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>331</v>
+        <v>239</v>
       </c>
       <c r="J85" s="6" t="s">
         <v>357</v>
@@ -4238,7 +4227,7 @@
     </row>
     <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B86" t="s">
         <v>236</v>
@@ -4250,7 +4239,7 @@
         <v>235</v>
       </c>
       <c r="E86" t="s">
-        <v>333</v>
+        <v>282</v>
       </c>
       <c r="F86" t="s">
         <v>126</v>
@@ -4262,7 +4251,7 @@
         <v>2011</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="J86" s="6" t="s">
         <v>357</v>
@@ -4270,19 +4259,19 @@
     </row>
     <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>70</v>
+        <v>332</v>
       </c>
       <c r="B87" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C87">
         <v>2011</v>
       </c>
       <c r="D87" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="E87" t="s">
-        <v>242</v>
+        <v>333</v>
       </c>
       <c r="F87" t="s">
         <v>126</v>
@@ -4294,7 +4283,7 @@
         <v>2011</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>243</v>
+        <v>334</v>
       </c>
       <c r="J87" s="6" t="s">
         <v>357</v>
@@ -4302,7 +4291,7 @@
     </row>
     <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>335</v>
+        <v>70</v>
       </c>
       <c r="B88" t="s">
         <v>240</v>
@@ -4314,7 +4303,7 @@
         <v>241</v>
       </c>
       <c r="E88" t="s">
-        <v>336</v>
+        <v>242</v>
       </c>
       <c r="F88" t="s">
         <v>126</v>
@@ -4325,8 +4314,8 @@
       <c r="H88">
         <v>2011</v>
       </c>
-      <c r="I88" s="4" t="s">
-        <v>337</v>
+      <c r="I88" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="J88" s="6" t="s">
         <v>357</v>
@@ -4334,31 +4323,31 @@
     </row>
     <row r="89" spans="1:10">
       <c r="A89" t="s">
-        <v>71</v>
+        <v>335</v>
       </c>
       <c r="B89" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C89">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="D89" t="s">
-        <v>200</v>
+        <v>241</v>
       </c>
       <c r="E89" t="s">
-        <v>245</v>
+        <v>336</v>
       </c>
       <c r="F89" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G89">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="H89">
-        <v>2014</v>
-      </c>
-      <c r="I89" s="1" t="s">
-        <v>246</v>
+        <v>2011</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>337</v>
       </c>
       <c r="J89" s="6" t="s">
         <v>357</v>
@@ -4366,19 +4355,19 @@
     </row>
     <row r="90" spans="1:10">
       <c r="A90" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B90" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C90">
         <v>2014</v>
       </c>
       <c r="D90" t="s">
-        <v>248</v>
+        <v>200</v>
       </c>
       <c r="E90" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F90" t="s">
         <v>105</v>
@@ -4390,7 +4379,7 @@
         <v>2014</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="J90" s="6" t="s">
         <v>357</v>
@@ -4398,7 +4387,7 @@
     </row>
     <row r="91" spans="1:10">
       <c r="A91" t="s">
-        <v>338</v>
+        <v>72</v>
       </c>
       <c r="B91" t="s">
         <v>247</v>
@@ -4410,7 +4399,7 @@
         <v>248</v>
       </c>
       <c r="E91" t="s">
-        <v>339</v>
+        <v>249</v>
       </c>
       <c r="F91" t="s">
         <v>105</v>
@@ -4422,7 +4411,7 @@
         <v>2014</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>340</v>
+        <v>250</v>
       </c>
       <c r="J91" s="6" t="s">
         <v>357</v>
@@ -4430,22 +4419,22 @@
     </row>
     <row r="92" spans="1:10">
       <c r="A92" t="s">
-        <v>73</v>
+        <v>338</v>
       </c>
       <c r="B92" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C92">
         <v>2014</v>
       </c>
       <c r="D92" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E92" t="s">
-        <v>253</v>
+        <v>339</v>
       </c>
       <c r="F92" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G92">
         <v>2014</v>
@@ -4454,15 +4443,15 @@
         <v>2014</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>254</v>
+        <v>340</v>
       </c>
       <c r="J92" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B93" t="s">
         <v>251</v>
@@ -4474,10 +4463,10 @@
         <v>252</v>
       </c>
       <c r="E93" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F93" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G93">
         <v>2014</v>
@@ -4486,7 +4475,7 @@
         <v>2014</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="J93" s="6" t="s">
         <v>358</v>
@@ -4494,7 +4483,7 @@
     </row>
     <row r="94" spans="1:10">
       <c r="A94" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B94" t="s">
         <v>251</v>
@@ -4506,7 +4495,7 @@
         <v>252</v>
       </c>
       <c r="E94" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F94" t="s">
         <v>105</v>
@@ -4518,7 +4507,7 @@
         <v>2014</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="J94" s="6" t="s">
         <v>358</v>
@@ -4526,7 +4515,7 @@
     </row>
     <row r="95" spans="1:10">
       <c r="A95" t="s">
-        <v>341</v>
+        <v>75</v>
       </c>
       <c r="B95" t="s">
         <v>251</v>
@@ -4538,10 +4527,10 @@
         <v>252</v>
       </c>
       <c r="E95" t="s">
-        <v>342</v>
+        <v>255</v>
       </c>
       <c r="F95" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G95">
         <v>2014</v>
@@ -4550,7 +4539,7 @@
         <v>2014</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>343</v>
+        <v>256</v>
       </c>
       <c r="J95" s="6" t="s">
         <v>358</v>
@@ -4558,42 +4547,42 @@
     </row>
     <row r="96" spans="1:10">
       <c r="A96" t="s">
-        <v>76</v>
+        <v>341</v>
       </c>
       <c r="B96" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C96">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="D96" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="E96" t="s">
-        <v>237</v>
+        <v>342</v>
       </c>
       <c r="F96" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G96">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="H96">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>261</v>
+        <v>343</v>
       </c>
       <c r="J96" s="6" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" t="s">
-        <v>344</v>
+        <v>76</v>
       </c>
       <c r="B97" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C97">
         <v>2016</v>
@@ -4602,7 +4591,7 @@
         <v>260</v>
       </c>
       <c r="E97" t="s">
-        <v>345</v>
+        <v>237</v>
       </c>
       <c r="F97" t="s">
         <v>105</v>
@@ -4613,16 +4602,16 @@
       <c r="H97">
         <v>2016</v>
       </c>
-      <c r="I97" s="4" t="s">
-        <v>346</v>
+      <c r="I97" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="J97" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" t="s">
-        <v>77</v>
+        <v>344</v>
       </c>
       <c r="B98" t="s">
         <v>262</v>
@@ -4634,7 +4623,7 @@
         <v>260</v>
       </c>
       <c r="E98" t="s">
-        <v>263</v>
+        <v>345</v>
       </c>
       <c r="F98" t="s">
         <v>105</v>
@@ -4645,8 +4634,8 @@
       <c r="H98">
         <v>2016</v>
       </c>
-      <c r="I98" s="1" t="s">
-        <v>264</v>
+      <c r="I98" s="4" t="s">
+        <v>346</v>
       </c>
       <c r="J98" s="6" t="s">
         <v>358</v>
@@ -4654,10 +4643,10 @@
     </row>
     <row r="99" spans="1:10">
       <c r="A99" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B99" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C99">
         <v>2016</v>
@@ -4666,7 +4655,7 @@
         <v>260</v>
       </c>
       <c r="E99" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F99" t="s">
         <v>105</v>
@@ -4678,15 +4667,15 @@
         <v>2016</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J99" s="6" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" t="s">
-        <v>362</v>
+        <v>78</v>
       </c>
       <c r="B100" t="s">
         <v>265</v>
@@ -4698,7 +4687,7 @@
         <v>260</v>
       </c>
       <c r="E100" t="s">
-        <v>319</v>
+        <v>266</v>
       </c>
       <c r="F100" t="s">
         <v>105</v>
@@ -4709,8 +4698,8 @@
       <c r="H100">
         <v>2016</v>
       </c>
-      <c r="I100" s="4" t="s">
-        <v>347</v>
+      <c r="I100" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="J100" s="6" t="s">
         <v>357</v>
@@ -4718,7 +4707,7 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="B101" t="s">
         <v>265</v>
@@ -4730,10 +4719,10 @@
         <v>260</v>
       </c>
       <c r="E101" t="s">
-        <v>349</v>
+        <v>319</v>
       </c>
       <c r="F101" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G101">
         <v>2016</v>
@@ -4741,8 +4730,8 @@
       <c r="H101">
         <v>2016</v>
       </c>
-      <c r="I101" s="1" t="s">
-        <v>350</v>
+      <c r="I101" s="4" t="s">
+        <v>347</v>
       </c>
       <c r="J101" s="6" t="s">
         <v>357</v>
@@ -4750,22 +4739,22 @@
     </row>
     <row r="102" spans="1:10">
       <c r="A102" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B102" t="s">
-        <v>352</v>
+        <v>265</v>
       </c>
       <c r="C102">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="D102" t="s">
-        <v>353</v>
+        <v>260</v>
       </c>
       <c r="E102" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F102" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G102">
         <v>2016</v>
@@ -4773,63 +4762,63 @@
       <c r="H102">
         <v>2016</v>
       </c>
-      <c r="I102" s="4" t="s">
-        <v>355</v>
+      <c r="I102" s="1" t="s">
+        <v>350</v>
       </c>
       <c r="J102" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" t="s">
-        <v>79</v>
+        <v>351</v>
       </c>
       <c r="B103" t="s">
-        <v>268</v>
+        <v>352</v>
       </c>
       <c r="C103">
-        <v>1952</v>
+        <v>2018</v>
       </c>
       <c r="D103" t="s">
-        <v>214</v>
+        <v>353</v>
       </c>
       <c r="E103" t="s">
-        <v>269</v>
+        <v>354</v>
       </c>
       <c r="F103" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G103">
-        <v>1952</v>
+        <v>2016</v>
       </c>
       <c r="H103">
-        <v>1952</v>
-      </c>
-      <c r="I103" s="1" t="s">
-        <v>270</v>
+        <v>2016</v>
+      </c>
+      <c r="I103" s="4" t="s">
+        <v>355</v>
       </c>
       <c r="J103" s="6" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="104" spans="1:10">
       <c r="A104" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B104" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C104">
         <v>1952</v>
       </c>
       <c r="D104" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
       <c r="E104" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F104" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G104">
         <v>1952</v>
@@ -4838,15 +4827,15 @@
         <v>1952</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="J104" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B105" t="s">
         <v>271</v>
@@ -4858,7 +4847,7 @@
         <v>248</v>
       </c>
       <c r="E105" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F105" t="s">
         <v>105</v>
@@ -4870,7 +4859,7 @@
         <v>1952</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="J105" s="6" t="s">
         <v>358</v>
@@ -4878,22 +4867,22 @@
     </row>
     <row r="106" spans="1:10">
       <c r="A106" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B106" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C106">
         <v>1952</v>
       </c>
       <c r="D106" t="s">
-        <v>200</v>
+        <v>248</v>
       </c>
       <c r="E106" t="s">
-        <v>125</v>
+        <v>275</v>
       </c>
       <c r="F106" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G106">
         <v>1952</v>
@@ -4902,27 +4891,27 @@
         <v>1952</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="J106" s="6" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B107" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C107">
         <v>1952</v>
       </c>
       <c r="D107" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="E107" t="s">
-        <v>279</v>
+        <v>125</v>
       </c>
       <c r="F107" t="s">
         <v>126</v>
@@ -4934,7 +4923,7 @@
         <v>1952</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="J107" s="6" t="s">
         <v>357</v>
@@ -4942,10 +4931,10 @@
     </row>
     <row r="108" spans="1:10">
       <c r="A108" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B108" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C108">
         <v>1952</v>
@@ -4954,7 +4943,7 @@
         <v>214</v>
       </c>
       <c r="E108" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F108" t="s">
         <v>126</v>
@@ -4966,7 +4955,7 @@
         <v>1952</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="J108" s="6" t="s">
         <v>357</v>
@@ -4974,19 +4963,19 @@
     </row>
     <row r="109" spans="1:10">
       <c r="A109" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B109" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C109">
         <v>1952</v>
       </c>
       <c r="D109" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
       <c r="E109" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F109" t="s">
         <v>126</v>
@@ -4998,7 +4987,7 @@
         <v>1952</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="J109" s="6" t="s">
         <v>357</v>
@@ -5006,22 +4995,22 @@
     </row>
     <row r="110" spans="1:10">
       <c r="A110" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B110" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C110">
         <v>1952</v>
       </c>
       <c r="D110" t="s">
-        <v>288</v>
+        <v>248</v>
       </c>
       <c r="E110" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F110" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G110">
         <v>1952</v>
@@ -5030,14 +5019,46 @@
         <v>1952</v>
       </c>
       <c r="I110" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="J110" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" t="s">
+        <v>86</v>
+      </c>
+      <c r="B111" t="s">
+        <v>287</v>
+      </c>
+      <c r="C111">
+        <v>1952</v>
+      </c>
+      <c r="D111" t="s">
+        <v>288</v>
+      </c>
+      <c r="E111" t="s">
+        <v>289</v>
+      </c>
+      <c r="F111" t="s">
+        <v>105</v>
+      </c>
+      <c r="G111">
+        <v>1952</v>
+      </c>
+      <c r="H111">
+        <v>1952</v>
+      </c>
+      <c r="I111" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="J110" s="6" t="s">
+      <c r="J111" s="6" t="s">
         <v>358</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I110">
+  <autoFilter ref="A1:I111">
     <filterColumn colId="1"/>
   </autoFilter>
   <hyperlinks>
@@ -5091,41 +5112,41 @@
     <hyperlink ref="I66" r:id="rId48"/>
     <hyperlink ref="I67" r:id="rId49"/>
     <hyperlink ref="I68" r:id="rId50"/>
-    <hyperlink ref="I71" r:id="rId51"/>
-    <hyperlink ref="I75" r:id="rId52"/>
-    <hyperlink ref="I76" r:id="rId53"/>
-    <hyperlink ref="I78" r:id="rId54"/>
-    <hyperlink ref="I83" r:id="rId55"/>
-    <hyperlink ref="I84" r:id="rId56"/>
-    <hyperlink ref="I87" r:id="rId57"/>
-    <hyperlink ref="I89" r:id="rId58"/>
-    <hyperlink ref="I90" r:id="rId59"/>
-    <hyperlink ref="I92" r:id="rId60"/>
-    <hyperlink ref="I94" r:id="rId61"/>
-    <hyperlink ref="I93" r:id="rId62"/>
-    <hyperlink ref="I96" r:id="rId63"/>
-    <hyperlink ref="I98" r:id="rId64"/>
-    <hyperlink ref="I99" r:id="rId65"/>
-    <hyperlink ref="I103" r:id="rId66"/>
-    <hyperlink ref="I105" r:id="rId67"/>
-    <hyperlink ref="I104" r:id="rId68"/>
-    <hyperlink ref="I106" r:id="rId69"/>
-    <hyperlink ref="I107" r:id="rId70"/>
-    <hyperlink ref="I108" r:id="rId71"/>
-    <hyperlink ref="I109" r:id="rId72"/>
-    <hyperlink ref="I110" r:id="rId73"/>
+    <hyperlink ref="I72" r:id="rId51"/>
+    <hyperlink ref="I76" r:id="rId52"/>
+    <hyperlink ref="I77" r:id="rId53"/>
+    <hyperlink ref="I79" r:id="rId54"/>
+    <hyperlink ref="I84" r:id="rId55"/>
+    <hyperlink ref="I85" r:id="rId56"/>
+    <hyperlink ref="I88" r:id="rId57"/>
+    <hyperlink ref="I90" r:id="rId58"/>
+    <hyperlink ref="I91" r:id="rId59"/>
+    <hyperlink ref="I93" r:id="rId60"/>
+    <hyperlink ref="I95" r:id="rId61"/>
+    <hyperlink ref="I94" r:id="rId62"/>
+    <hyperlink ref="I97" r:id="rId63"/>
+    <hyperlink ref="I99" r:id="rId64"/>
+    <hyperlink ref="I100" r:id="rId65"/>
+    <hyperlink ref="I104" r:id="rId66"/>
+    <hyperlink ref="I106" r:id="rId67"/>
+    <hyperlink ref="I105" r:id="rId68"/>
+    <hyperlink ref="I107" r:id="rId69"/>
+    <hyperlink ref="I108" r:id="rId70"/>
+    <hyperlink ref="I109" r:id="rId71"/>
+    <hyperlink ref="I110" r:id="rId72"/>
+    <hyperlink ref="I111" r:id="rId73"/>
     <hyperlink ref="I44" r:id="rId74"/>
-    <hyperlink ref="I81" r:id="rId75"/>
+    <hyperlink ref="I82" r:id="rId75"/>
     <hyperlink ref="I4" r:id="rId76"/>
     <hyperlink ref="I25" r:id="rId77"/>
     <hyperlink ref="I61" r:id="rId78"/>
     <hyperlink ref="I57" r:id="rId79"/>
-    <hyperlink ref="I80" r:id="rId80"/>
-    <hyperlink ref="I85" r:id="rId81"/>
-    <hyperlink ref="I86" r:id="rId82"/>
-    <hyperlink ref="I91" r:id="rId83"/>
-    <hyperlink ref="I95" r:id="rId84"/>
-    <hyperlink ref="I101" r:id="rId85"/>
+    <hyperlink ref="I81" r:id="rId80"/>
+    <hyperlink ref="I86" r:id="rId81"/>
+    <hyperlink ref="I87" r:id="rId82"/>
+    <hyperlink ref="I92" r:id="rId83"/>
+    <hyperlink ref="I96" r:id="rId84"/>
+    <hyperlink ref="I102" r:id="rId85"/>
     <hyperlink ref="I45" r:id="rId86"/>
     <hyperlink ref="I46" r:id="rId87"/>
     <hyperlink ref="I42" r:id="rId88"/>

</xml_diff>

<commit_message>
update all source files
</commit_message>
<xml_diff>
--- a/corpus/evenki/current_meta.xlsx
+++ b/corpus/evenki/current_meta.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="387">
   <si>
     <t>filename</t>
   </si>
@@ -1176,6 +1176,21 @@
   </si>
   <si>
     <t>2007_Mutoray_Yastrikova_FSk5_transliterated</t>
+  </si>
+  <si>
+    <t>2019_Torom_MalyshevAF_LF5_transliterated</t>
+  </si>
+  <si>
+    <t>Малышев Алексей Федорович</t>
+  </si>
+  <si>
+    <t>Тором</t>
+  </si>
+  <si>
+    <t>Кто-то черный</t>
+  </si>
+  <si>
+    <t>http://siberian-lang.srcc.msu.ru/ru/node/4889464</t>
   </si>
 </sst>
 </file>
@@ -1562,11 +1577,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J111"/>
+  <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -5074,6 +5087,38 @@
         <v>290</v>
       </c>
       <c r="J111" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112" t="s">
+        <v>382</v>
+      </c>
+      <c r="B112" t="s">
+        <v>383</v>
+      </c>
+      <c r="C112">
+        <v>2019</v>
+      </c>
+      <c r="D112" t="s">
+        <v>384</v>
+      </c>
+      <c r="E112" t="s">
+        <v>385</v>
+      </c>
+      <c r="F112" t="s">
+        <v>105</v>
+      </c>
+      <c r="G112">
+        <v>2019</v>
+      </c>
+      <c r="H112">
+        <v>2019</v>
+      </c>
+      <c r="I112" t="s">
+        <v>386</v>
+      </c>
+      <c r="J112" s="6" t="s">
         <v>358</v>
       </c>
     </row>

</xml_diff>